<commit_message>
Morning Update - RW Updates
Rw- Kolkata ,
Halted due to Act of  Violation From
Puthiyathalaimurai TV , AajTak & TCS

No RW Business Rights to above Institution & their Employees
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO-PC\OneDrive\Documents\Work_For_\Work\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CEE7487-A707-4014-8472-55E6CB14A9E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E161D6F0-521F-454A-9D14-60CFC429C880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="554" uniqueCount="134">
   <si>
     <t>UnSettled</t>
   </si>
@@ -416,9 +416,6 @@
     <t>TBS</t>
   </si>
   <si>
-    <t>Food - SS MgX</t>
-  </si>
-  <si>
     <t>pp</t>
   </si>
   <si>
@@ -435,6 +432,12 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>Food - Cheat</t>
+  </si>
+  <si>
+    <t>Zee 24 Taas</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1160,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="170">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1438,6 +1441,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1456,97 +1474,89 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1830,7 +1840,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:O15"/>
+      <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1864,7 +1874,7 @@
       <c r="B2" s="35">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="132">
+      <c r="C2" s="137">
         <f>B3+B4</f>
         <v>2175</v>
       </c>
@@ -1897,7 +1907,7 @@
         <v>68</v>
       </c>
       <c r="O2" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="P2" s="91" t="s">
         <v>83</v>
@@ -1910,23 +1920,23 @@
       </c>
       <c r="T2" s="100">
         <f ca="1">TODAY()</f>
-        <v>45274</v>
+        <v>45275</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="130" t="s">
+      <c r="A3" s="135" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="35">
         <v>2000</v>
       </c>
-      <c r="C3" s="133"/>
+      <c r="C3" s="138"/>
       <c r="D3" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="131"/>
+      <c r="A4" s="136"/>
       <c r="B4" s="35">
         <v>175</v>
       </c>
@@ -1934,15 +1944,13 @@
         <v>35</v>
       </c>
       <c r="E4" s="34">
-        <v>15</v>
-      </c>
-      <c r="F4" s="39">
-        <v>20</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F4" s="39"/>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="125" t="s">
+      <c r="H4" s="109" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="120" t="s">
@@ -1961,7 +1969,7 @@
         <v>30</v>
       </c>
       <c r="N4" s="80">
-        <v>0.5083333333333333</v>
+        <v>0.38125000000000003</v>
       </c>
       <c r="P4" s="80">
         <v>0.78472222222222221</v>
@@ -1975,15 +1983,13 @@
         <v>-2</v>
       </c>
       <c r="E5" s="34">
-        <v>25</v>
-      </c>
-      <c r="F5" s="157">
-        <v>10</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="F5" s="128"/>
       <c r="G5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="H5" s="108" t="s">
+      <c r="H5" s="109" t="s">
         <v>17</v>
       </c>
       <c r="I5" s="85" t="s">
@@ -1996,13 +2002,13 @@
         <v>119</v>
       </c>
       <c r="L5" s="30" t="s">
-        <v>85</v>
+        <v>124</v>
       </c>
       <c r="M5" s="30" t="s">
         <v>86</v>
       </c>
       <c r="N5" s="80">
-        <v>0.5083333333333333</v>
+        <v>0.38125000000000003</v>
       </c>
       <c r="P5" s="80">
         <v>0.53472222222222221</v>
@@ -2013,13 +2019,11 @@
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="34">
-        <v>40</v>
-      </c>
-      <c r="F6" s="158">
         <v>10</v>
       </c>
+      <c r="F6" s="129"/>
       <c r="G6" s="28" t="s">
-        <v>126</v>
+        <v>132</v>
       </c>
       <c r="H6" s="122" t="s">
         <v>17</v>
@@ -2034,16 +2038,16 @@
         <v>120</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="M6" s="30" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="N6" s="80">
-        <v>0.5083333333333333</v>
+        <v>0.38125000000000003</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="P6" s="80">
         <v>0.5083333333333333</v>
@@ -2059,12 +2063,8 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="34">
-        <v>1</v>
-      </c>
-      <c r="F7" s="158">
-        <v>10</v>
-      </c>
+      <c r="E7" s="34"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2081,16 +2081,16 @@
         <v>121</v>
       </c>
       <c r="L7" s="30" t="s">
-        <v>124</v>
+        <v>21</v>
       </c>
       <c r="M7" s="30" t="s">
         <v>90</v>
       </c>
       <c r="N7" s="80">
-        <v>0.78472222222222221</v>
+        <v>0.38125000000000003</v>
       </c>
       <c r="P7" s="80">
-        <v>0.5083333333333333</v>
+        <v>0.38125000000000003</v>
       </c>
       <c r="R7" s="25" t="s">
         <v>112</v>
@@ -2098,9 +2098,7 @@
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="34"/>
-      <c r="F8" s="39">
-        <v>50</v>
-      </c>
+      <c r="F8" s="39"/>
       <c r="G8" s="9" t="s">
         <v>72</v>
       </c>
@@ -2141,13 +2139,11 @@
         <v>4825</v>
       </c>
       <c r="E9" s="34"/>
-      <c r="F9" s="157">
-        <v>10</v>
-      </c>
+      <c r="F9" s="128"/>
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="160" t="s">
+      <c r="H9" s="131" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="120" t="s">
@@ -2169,22 +2165,18 @@
         <v>0.78472222222222221</v>
       </c>
       <c r="O9" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="P9" s="80">
         <v>0.78472222222222221</v>
       </c>
       <c r="R9" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="34">
-        <v>49</v>
-      </c>
-      <c r="F10" s="39">
-        <v>70</v>
-      </c>
+      <c r="E10" s="34"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="9" t="s">
         <v>81</v>
       </c>
@@ -2213,7 +2205,7 @@
         <v>0.78472222222222221</v>
       </c>
       <c r="R10" s="25" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2224,12 +2216,10 @@
         <f>B9-B13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="159"/>
-      <c r="F11" s="39">
-        <v>55</v>
-      </c>
+      <c r="E11" s="130"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H11" s="109" t="s">
         <v>17</v>
@@ -2240,8 +2230,8 @@
       <c r="J11" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="K11" s="154" t="s">
-        <v>130</v>
+      <c r="K11" s="9" t="s">
+        <v>129</v>
       </c>
       <c r="L11" s="24" t="s">
         <v>62</v>
@@ -2252,15 +2242,18 @@
       <c r="N11" s="80">
         <v>0.78472222222222221</v>
       </c>
+      <c r="R11" s="25" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="155" t="s">
+      <c r="E12" s="139" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="156"/>
+      <c r="F12" s="140"/>
       <c r="G12" s="9">
-        <f>SUM(E4:E10)</f>
-        <v>130</v>
+        <f>SUM(E4:F11)</f>
+        <v>40</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
@@ -2277,12 +2270,12 @@
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="121"/>
-      <c r="J13" s="128"/>
+      <c r="J13" s="133"/>
       <c r="K13" s="25"/>
       <c r="L13"/>
       <c r="M13"/>
-      <c r="N13" s="129"/>
-      <c r="O13" s="129"/>
+      <c r="N13" s="134"/>
+      <c r="O13" s="134"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
@@ -2290,11 +2283,11 @@
       <c r="E14" s="24"/>
       <c r="F14" s="20"/>
       <c r="I14" s="121"/>
-      <c r="J14" s="128"/>
+      <c r="J14" s="133"/>
       <c r="L14"/>
       <c r="M14"/>
-      <c r="N14" s="129"/>
-      <c r="O14" s="129"/>
+      <c r="N14" s="134"/>
+      <c r="O14" s="134"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2308,11 +2301,11 @@
       <c r="E15" s="24"/>
       <c r="F15" s="20"/>
       <c r="I15" s="121"/>
-      <c r="J15" s="128"/>
+      <c r="J15" s="133"/>
       <c r="L15"/>
       <c r="M15"/>
-      <c r="N15" s="129"/>
-      <c r="O15" s="129"/>
+      <c r="N15" s="134"/>
+      <c r="O15" s="134"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="25"/>
@@ -2331,8 +2324,8 @@
       <c r="I17" s="121"/>
       <c r="L17"/>
       <c r="M17"/>
-      <c r="N17" s="129"/>
-      <c r="O17" s="129"/>
+      <c r="N17" s="134"/>
+      <c r="O17" s="134"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2345,14 +2338,14 @@
       <c r="D18" s="25"/>
       <c r="E18" s="24"/>
       <c r="F18" s="20"/>
-      <c r="J18" s="128"/>
+      <c r="J18" s="133"/>
       <c r="L18"/>
       <c r="M18"/>
-      <c r="N18" s="129"/>
-      <c r="O18" s="129"/>
+      <c r="N18" s="134"/>
+      <c r="O18" s="134"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J19" s="128"/>
+      <c r="J19" s="133"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
@@ -2374,10 +2367,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2400,18 +2393,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="140" t="s">
+      <c r="E1" s="148" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="141"/>
+      <c r="F1" s="149"/>
       <c r="G1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="140" t="s">
+      <c r="H1" s="148" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="142"/>
-      <c r="J1" s="141"/>
+      <c r="I1" s="150"/>
+      <c r="J1" s="149"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2429,7 +2422,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="136">
+      <c r="B2" s="143">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2456,15 +2449,15 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="144">
+      <c r="K2" s="151">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="146">
+      <c r="L2" s="153">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="138">
+      <c r="M2" s="146">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
@@ -2475,7 +2468,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="137"/>
+      <c r="B3" s="145"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2490,13 +2483,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="57"/>
-      <c r="K3" s="145"/>
-      <c r="L3" s="147"/>
-      <c r="M3" s="139"/>
+      <c r="K3" s="152"/>
+      <c r="L3" s="154"/>
+      <c r="M3" s="147"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="143"/>
+      <c r="B4" s="144"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2511,9 +2504,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="145"/>
-      <c r="L4" s="147"/>
-      <c r="M4" s="139"/>
+      <c r="K4" s="152"/>
+      <c r="L4" s="154"/>
+      <c r="M4" s="147"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2595,7 +2588,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="134">
+      <c r="B7" s="155">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2612,22 +2605,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="148">
+      <c r="K7" s="157">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="150">
+      <c r="L7" s="159">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="152">
+      <c r="M7" s="161">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="135"/>
+      <c r="B8" s="156"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2648,9 +2641,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="149"/>
-      <c r="L8" s="151"/>
-      <c r="M8" s="153"/>
+      <c r="K8" s="158"/>
+      <c r="L8" s="160"/>
+      <c r="M8" s="162"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2730,7 +2723,7 @@
       <c r="A11" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="134">
+      <c r="B11" s="155">
         <v>8</v>
       </c>
       <c r="C11" s="70"/>
@@ -2757,7 +2750,7 @@
       <c r="M11" s="72"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="135"/>
+      <c r="B12" s="156"/>
       <c r="C12" s="92">
         <v>483</v>
       </c>
@@ -2814,7 +2807,7 @@
       <c r="M13" s="84"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="134">
+      <c r="B14" s="155">
         <v>10</v>
       </c>
       <c r="C14" s="97"/>
@@ -2837,7 +2830,7 @@
       <c r="A15" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="135"/>
+      <c r="B15" s="156"/>
       <c r="C15" s="98"/>
       <c r="D15" s="84">
         <v>175</v>
@@ -2861,7 +2854,7 @@
       <c r="M15" s="93"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="136">
+      <c r="B16" s="143">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -2892,7 +2885,7 @@
       <c r="A17" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="137"/>
+      <c r="B17" s="145"/>
       <c r="C17" s="84"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
@@ -2910,7 +2903,7 @@
       <c r="M17" s="84"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="136">
+      <c r="B18" s="143">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -2939,7 +2932,7 @@
       <c r="A19" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="143"/>
+      <c r="B19" s="144"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -2964,7 +2957,7 @@
       <c r="A20" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="161">
+      <c r="B20" s="132">
         <v>13</v>
       </c>
       <c r="C20" s="13"/>
@@ -2999,7 +2992,7 @@
       <c r="A21" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="165">
+      <c r="B21" s="141">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3027,32 +3020,56 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="166"/>
-      <c r="C22" s="162"/>
-      <c r="D22" s="163">
+      <c r="B22" s="142"/>
+      <c r="C22" s="163"/>
+      <c r="D22" s="164">
         <v>235</v>
       </c>
-      <c r="E22" s="163">
+      <c r="E22" s="164">
         <v>50</v>
       </c>
-      <c r="F22" s="163">
+      <c r="F22" s="164">
         <v>55</v>
       </c>
-      <c r="G22" s="163">
+      <c r="G22" s="164">
         <v>70</v>
       </c>
-      <c r="H22" s="157">
+      <c r="H22" s="165">
         <v>20</v>
       </c>
-      <c r="I22" s="163">
+      <c r="I22" s="164">
         <v>20</v>
       </c>
-      <c r="J22" s="158">
+      <c r="J22" s="166">
         <v>20</v>
       </c>
-      <c r="K22" s="163"/>
-      <c r="L22" s="163"/>
-      <c r="M22" s="164"/>
+      <c r="K22" s="164"/>
+      <c r="L22" s="164"/>
+      <c r="M22" s="167"/>
+    </row>
+    <row r="23" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="79">
+        <v>15</v>
+      </c>
+      <c r="C23" s="58"/>
+      <c r="D23" s="169">
+        <v>40</v>
+      </c>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="168">
+        <v>20</v>
+      </c>
+      <c r="I23" s="168">
+        <v>10</v>
+      </c>
+      <c r="J23" s="168">
+        <v>10</v>
+      </c>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="15">
@@ -4630,7 +4647,7 @@
       </c>
       <c r="AD14" s="100">
         <f ca="1">TODAY()</f>
-        <v>45274</v>
+        <v>45275</v>
       </c>
     </row>
     <row r="15" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Rw - Chennai Update
Food - SS - MgX
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38DCCF9F-4355-449F-B8E2-5F8D97615034}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00B95AC-1FF1-4B26-B32B-A8E6F153A3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="137">
   <si>
     <t>UnSettled</t>
   </si>
@@ -440,10 +440,13 @@
     <t>Zee 24 Taas</t>
   </si>
   <si>
+    <t>17/12/2023</t>
+  </si>
+  <si>
     <t xml:space="preserve">Food </t>
   </si>
   <si>
-    <t>17/12/2023</t>
+    <t>Food- SS MgX</t>
   </si>
 </sst>
 </file>
@@ -1174,7 +1177,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="184">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1479,6 +1482,20 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1567,42 +1584,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1888,7 +1869,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1922,7 +1903,7 @@
       <c r="B2" s="35">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="142">
+      <c r="C2" s="148">
         <f>B3+B4</f>
         <v>1930</v>
       </c>
@@ -1972,19 +1953,19 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="140" t="s">
+      <c r="A3" s="146" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="35">
         <v>1500</v>
       </c>
-      <c r="C3" s="143"/>
+      <c r="C3" s="149"/>
       <c r="D3" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="141"/>
+      <c r="A4" s="147"/>
       <c r="B4" s="35">
         <v>430</v>
       </c>
@@ -2035,7 +2016,7 @@
       </c>
       <c r="F5" s="128"/>
       <c r="G5" s="9" t="s">
-        <v>1</v>
+        <v>136</v>
       </c>
       <c r="H5" s="109" t="s">
         <v>17</v>
@@ -2071,7 +2052,7 @@
       </c>
       <c r="F6" s="129"/>
       <c r="G6" s="28" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H6" s="122" t="s">
         <v>17</v>
@@ -2111,7 +2092,7 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="183">
+      <c r="E7" s="143">
         <v>3</v>
       </c>
       <c r="F7" s="129"/>
@@ -2179,7 +2160,7 @@
         <v>0.55625000000000002</v>
       </c>
       <c r="R8" s="25" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2272,7 +2253,7 @@
         <f>B9-B13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="183">
+      <c r="E11" s="143">
         <v>2</v>
       </c>
       <c r="F11" s="39"/>
@@ -2308,10 +2289,10 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="144" t="s">
+      <c r="E12" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="145"/>
+      <c r="F12" s="151"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
         <v>205</v>
@@ -2331,11 +2312,11 @@
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="121"/>
-      <c r="J13" s="138"/>
+      <c r="J13" s="144"/>
       <c r="L13"/>
       <c r="M13"/>
-      <c r="N13" s="139"/>
-      <c r="O13" s="139"/>
+      <c r="N13" s="145"/>
+      <c r="O13" s="145"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
@@ -2343,11 +2324,11 @@
       <c r="E14" s="24"/>
       <c r="F14" s="20"/>
       <c r="I14" s="121"/>
-      <c r="J14" s="138"/>
+      <c r="J14" s="144"/>
       <c r="L14"/>
       <c r="M14"/>
-      <c r="N14" s="139"/>
-      <c r="O14" s="139"/>
+      <c r="N14" s="145"/>
+      <c r="O14" s="145"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2361,12 +2342,12 @@
       <c r="E15" s="24"/>
       <c r="F15" s="20"/>
       <c r="I15" s="121"/>
-      <c r="J15" s="138"/>
+      <c r="J15" s="144"/>
       <c r="K15" s="121"/>
       <c r="L15"/>
       <c r="M15"/>
-      <c r="N15" s="139"/>
-      <c r="O15" s="139"/>
+      <c r="N15" s="145"/>
+      <c r="O15" s="145"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="25"/>
@@ -2385,8 +2366,8 @@
       <c r="I17" s="121"/>
       <c r="L17"/>
       <c r="M17"/>
-      <c r="N17" s="139"/>
-      <c r="O17" s="139"/>
+      <c r="N17" s="145"/>
+      <c r="O17" s="145"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2399,14 +2380,14 @@
       <c r="D18" s="25"/>
       <c r="E18" s="24"/>
       <c r="F18" s="20"/>
-      <c r="J18" s="138"/>
+      <c r="J18" s="144"/>
       <c r="L18"/>
       <c r="M18"/>
-      <c r="N18" s="139"/>
-      <c r="O18" s="139"/>
+      <c r="N18" s="145"/>
+      <c r="O18" s="145"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J19" s="138"/>
+      <c r="J19" s="144"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
@@ -2454,18 +2435,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="153" t="s">
+      <c r="E1" s="159" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="154"/>
+      <c r="F1" s="160"/>
       <c r="G1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="153" t="s">
+      <c r="H1" s="159" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="155"/>
-      <c r="J1" s="154"/>
+      <c r="I1" s="161"/>
+      <c r="J1" s="160"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2483,7 +2464,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="148">
+      <c r="B2" s="154">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2510,15 +2491,15 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="156">
+      <c r="K2" s="162">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="158">
+      <c r="L2" s="164">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="151">
+      <c r="M2" s="157">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
@@ -2529,7 +2510,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="150"/>
+      <c r="B3" s="156"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2544,13 +2525,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="57"/>
-      <c r="K3" s="157"/>
-      <c r="L3" s="159"/>
-      <c r="M3" s="152"/>
+      <c r="K3" s="163"/>
+      <c r="L3" s="165"/>
+      <c r="M3" s="158"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="149"/>
+      <c r="B4" s="155"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2565,9 +2546,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="157"/>
-      <c r="L4" s="159"/>
-      <c r="M4" s="152"/>
+      <c r="K4" s="163"/>
+      <c r="L4" s="165"/>
+      <c r="M4" s="158"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2649,7 +2630,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="160">
+      <c r="B7" s="166">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2666,22 +2647,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="162">
+      <c r="K7" s="168">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="164">
+      <c r="L7" s="170">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="166">
+      <c r="M7" s="172">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="161"/>
+      <c r="B8" s="167"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2702,9 +2683,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="163"/>
-      <c r="L8" s="165"/>
-      <c r="M8" s="167"/>
+      <c r="K8" s="169"/>
+      <c r="L8" s="171"/>
+      <c r="M8" s="173"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2784,7 +2765,7 @@
       <c r="A11" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="160">
+      <c r="B11" s="166">
         <v>8</v>
       </c>
       <c r="C11" s="70"/>
@@ -2811,7 +2792,7 @@
       <c r="M11" s="72"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="161"/>
+      <c r="B12" s="167"/>
       <c r="C12" s="92">
         <v>483</v>
       </c>
@@ -2868,7 +2849,7 @@
       <c r="M13" s="84"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="160">
+      <c r="B14" s="166">
         <v>10</v>
       </c>
       <c r="C14" s="97"/>
@@ -2891,7 +2872,7 @@
       <c r="A15" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="161"/>
+      <c r="B15" s="167"/>
       <c r="C15" s="98"/>
       <c r="D15" s="84">
         <v>175</v>
@@ -2915,7 +2896,7 @@
       <c r="M15" s="93"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="148">
+      <c r="B16" s="154">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -2946,7 +2927,7 @@
       <c r="A17" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="150"/>
+      <c r="B17" s="156"/>
       <c r="C17" s="84"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
@@ -2964,7 +2945,7 @@
       <c r="M17" s="84"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="148">
+      <c r="B18" s="154">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -2993,7 +2974,7 @@
       <c r="A19" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="149"/>
+      <c r="B19" s="155"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3053,7 +3034,7 @@
       <c r="A21" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="146">
+      <c r="B21" s="152">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3081,7 +3062,7 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="147"/>
+      <c r="B22" s="153"/>
       <c r="C22" s="133"/>
       <c r="D22" s="134">
         <v>235</v>
@@ -3113,7 +3094,7 @@
         <v>15</v>
       </c>
       <c r="C23" s="70"/>
-      <c r="D23" s="180">
+      <c r="D23" s="141">
         <v>40</v>
       </c>
       <c r="E23" s="71"/>
@@ -3139,16 +3120,16 @@
       <c r="C24" s="58"/>
       <c r="D24" s="59"/>
       <c r="E24" s="59"/>
-      <c r="F24" s="181">
+      <c r="F24" s="59">
         <v>75</v>
       </c>
-      <c r="G24" s="181">
+      <c r="G24" s="59">
         <v>70</v>
       </c>
-      <c r="H24" s="181">
+      <c r="H24" s="59">
         <v>30</v>
       </c>
-      <c r="I24" s="182">
+      <c r="I24" s="142">
         <v>5</v>
       </c>
       <c r="J24" s="59">
@@ -4800,34 +4781,27 @@
       <c r="L15" s="25"/>
       <c r="M15" s="24"/>
       <c r="N15" s="103"/>
-      <c r="P15" s="168"/>
-      <c r="Q15" s="169"/>
-      <c r="R15" s="170"/>
-      <c r="S15" s="171"/>
-      <c r="T15" s="172"/>
-      <c r="U15" s="169"/>
-      <c r="V15" s="173"/>
-      <c r="W15" s="173"/>
-      <c r="X15" s="173"/>
-      <c r="Y15" s="173"/>
-      <c r="Z15" s="169"/>
-      <c r="AA15" s="173"/>
+      <c r="P15" s="138"/>
+      <c r="R15" s="25"/>
+      <c r="S15" s="119"/>
+      <c r="T15" s="2"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="AA15" s="1"/>
       <c r="AB15" s="103"/>
-      <c r="AG15" s="168"/>
-      <c r="AH15" s="172"/>
-      <c r="AI15" s="169"/>
-      <c r="AJ15" s="170"/>
-      <c r="AK15" s="171"/>
-      <c r="AL15" s="172"/>
-      <c r="AM15" s="169"/>
-      <c r="AN15" s="173"/>
-      <c r="AO15" s="173"/>
-      <c r="AP15" s="173"/>
-      <c r="AQ15" s="173"/>
-      <c r="AR15" s="169"/>
-      <c r="AS15" s="173"/>
-      <c r="AT15" s="170"/>
-      <c r="AU15" s="169"/>
+      <c r="AG15" s="138"/>
+      <c r="AH15" s="2"/>
+      <c r="AJ15" s="25"/>
+      <c r="AK15" s="119"/>
+      <c r="AL15" s="2"/>
+      <c r="AN15" s="1"/>
+      <c r="AO15" s="1"/>
+      <c r="AP15" s="1"/>
+      <c r="AQ15" s="1"/>
+      <c r="AS15" s="1"/>
+      <c r="AT15" s="25"/>
       <c r="AV15" s="51"/>
     </row>
     <row r="16" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4885,20 +4859,20 @@
       <c r="U16" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="V16" s="174" t="s">
+      <c r="V16" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="W16" s="174" t="s">
+      <c r="W16" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="X16" s="175">
+      <c r="X16" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="Y16" s="173"/>
-      <c r="Z16" s="175">
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="80">
         <v>0.61805555555555558</v>
       </c>
-      <c r="AA16" s="173"/>
+      <c r="AA16" s="1"/>
       <c r="AB16" s="103" t="s">
         <v>106</v>
       </c>
@@ -4921,24 +4895,23 @@
       <c r="AM16" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="AN16" s="174" t="s">
+      <c r="AN16" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="AO16" s="174" t="s">
+      <c r="AO16" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="AP16" s="175">
+      <c r="AP16" s="80">
         <v>0.38125000000000003</v>
       </c>
-      <c r="AQ16" s="173"/>
-      <c r="AR16" s="175">
+      <c r="AQ16" s="1"/>
+      <c r="AR16" s="80">
         <v>0.78472222222222221</v>
       </c>
-      <c r="AS16" s="173"/>
-      <c r="AT16" s="170" t="s">
+      <c r="AS16" s="1"/>
+      <c r="AT16" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="AU16" s="169"/>
       <c r="AV16" s="51"/>
     </row>
     <row r="17" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4998,20 +4971,20 @@
       <c r="U17" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="V17" s="174" t="s">
+      <c r="V17" s="30" t="s">
         <v>85</v>
       </c>
-      <c r="W17" s="174" t="s">
+      <c r="W17" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="X17" s="175">
+      <c r="X17" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="Y17" s="173"/>
-      <c r="Z17" s="175">
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="80">
         <v>0.53472222222222221</v>
       </c>
-      <c r="AA17" s="173"/>
+      <c r="AA17" s="1"/>
       <c r="AB17" s="103" t="s">
         <v>106</v>
       </c>
@@ -5034,24 +5007,23 @@
       <c r="AM17" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="AN17" s="174" t="s">
+      <c r="AN17" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="AO17" s="174" t="s">
+      <c r="AO17" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="AP17" s="175">
+      <c r="AP17" s="80">
         <v>0.38125000000000003</v>
       </c>
-      <c r="AQ17" s="173"/>
-      <c r="AR17" s="175">
+      <c r="AQ17" s="1"/>
+      <c r="AR17" s="80">
         <v>0.53472222222222221</v>
       </c>
-      <c r="AS17" s="173"/>
-      <c r="AT17" s="170" t="s">
+      <c r="AS17" s="1"/>
+      <c r="AT17" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="AU17" s="169"/>
       <c r="AV17" s="51"/>
     </row>
     <row r="18" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5094,7 +5066,7 @@
       <c r="P18" s="38">
         <v>5</v>
       </c>
-      <c r="Q18" s="176" t="s">
+      <c r="Q18" s="28" t="s">
         <v>9</v>
       </c>
       <c r="R18" s="122" t="s">
@@ -5109,20 +5081,20 @@
       <c r="U18" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="V18" s="174" t="s">
+      <c r="V18" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="W18" s="174" t="s">
+      <c r="W18" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="X18" s="175">
+      <c r="X18" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="Y18" s="173"/>
-      <c r="Z18" s="175">
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="AA18" s="173"/>
+      <c r="AA18" s="1"/>
       <c r="AB18" s="103" t="s">
         <v>106</v>
       </c>
@@ -5130,7 +5102,7 @@
         <v>10</v>
       </c>
       <c r="AH18" s="129"/>
-      <c r="AI18" s="176" t="s">
+      <c r="AI18" s="28" t="s">
         <v>132</v>
       </c>
       <c r="AJ18" s="122" t="s">
@@ -5145,26 +5117,25 @@
       <c r="AM18" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="AN18" s="174" t="s">
+      <c r="AN18" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="AO18" s="174" t="s">
+      <c r="AO18" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="AP18" s="175">
+      <c r="AP18" s="80">
         <v>0.38125000000000003</v>
       </c>
-      <c r="AQ18" s="173" t="s">
+      <c r="AQ18" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="AR18" s="175">
+      <c r="AR18" s="80">
         <v>0.5083333333333333</v>
       </c>
-      <c r="AS18" s="173"/>
-      <c r="AT18" s="170" t="s">
+      <c r="AS18" s="1"/>
+      <c r="AT18" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="AU18" s="169"/>
       <c r="AV18" s="51"/>
     </row>
     <row r="19" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5222,20 +5193,20 @@
       <c r="U19" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="V19" s="174" t="s">
+      <c r="V19" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="W19" s="174" t="s">
+      <c r="W19" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="X19" s="175">
+      <c r="X19" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="Y19" s="173"/>
-      <c r="Z19" s="175">
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="AA19" s="173"/>
+      <c r="AA19" s="1"/>
       <c r="AB19" s="103" t="s">
         <v>106</v>
       </c>
@@ -5256,24 +5227,23 @@
       <c r="AM19" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="AN19" s="174" t="s">
+      <c r="AN19" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="AO19" s="174" t="s">
+      <c r="AO19" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="AP19" s="175">
+      <c r="AP19" s="80">
         <v>0.38125000000000003</v>
       </c>
-      <c r="AQ19" s="173"/>
-      <c r="AR19" s="175">
+      <c r="AQ19" s="1"/>
+      <c r="AR19" s="80">
         <v>0.38125000000000003</v>
       </c>
-      <c r="AS19" s="173"/>
-      <c r="AT19" s="170" t="s">
+      <c r="AS19" s="1"/>
+      <c r="AT19" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="AU19" s="169"/>
       <c r="AV19" s="51"/>
     </row>
     <row r="20" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5331,20 +5301,20 @@
       <c r="U20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="V20" s="174" t="s">
+      <c r="V20" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="W20" s="174" t="s">
+      <c r="W20" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="X20" s="175">
+      <c r="X20" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="Y20" s="173"/>
-      <c r="Z20" s="175">
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="80">
         <v>0.53472222222222221</v>
       </c>
-      <c r="AA20" s="173"/>
+      <c r="AA20" s="1"/>
       <c r="AB20" s="103" t="s">
         <v>106</v>
       </c>
@@ -5365,24 +5335,23 @@
       <c r="AM20" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="AN20" s="174" t="s">
+      <c r="AN20" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="AO20" s="174" t="s">
+      <c r="AO20" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="AP20" s="175">
+      <c r="AP20" s="80">
         <v>0.78472222222222221</v>
       </c>
-      <c r="AQ20" s="173"/>
-      <c r="AR20" s="175">
+      <c r="AQ20" s="1"/>
+      <c r="AR20" s="80">
         <v>0.53472222222222221</v>
       </c>
-      <c r="AS20" s="173"/>
-      <c r="AT20" s="170" t="s">
+      <c r="AS20" s="1"/>
+      <c r="AT20" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="AU20" s="169"/>
       <c r="AV20" s="51"/>
     </row>
     <row r="21" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5440,20 +5409,20 @@
       <c r="U21" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="V21" s="174" t="s">
+      <c r="V21" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="W21" s="174" t="s">
+      <c r="W21" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="X21" s="175">
+      <c r="X21" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="Y21" s="173"/>
-      <c r="Z21" s="175">
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="AA21" s="173"/>
+      <c r="AA21" s="1"/>
       <c r="AB21" s="103" t="s">
         <v>112</v>
       </c>
@@ -5474,26 +5443,25 @@
       <c r="AM21" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="AN21" s="174" t="s">
+      <c r="AN21" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="AO21" s="174" t="s">
+      <c r="AO21" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="AP21" s="175">
+      <c r="AP21" s="80">
         <v>0.78472222222222221</v>
       </c>
-      <c r="AQ21" s="173" t="s">
+      <c r="AQ21" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="AR21" s="175">
+      <c r="AR21" s="80">
         <v>0.78472222222222221</v>
       </c>
-      <c r="AS21" s="173"/>
-      <c r="AT21" s="170" t="s">
+      <c r="AS21" s="1"/>
+      <c r="AT21" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="AU21" s="169"/>
       <c r="AV21" s="51"/>
     </row>
     <row r="22" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5551,20 +5519,20 @@
       <c r="U22" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="V22" s="174" t="s">
+      <c r="V22" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="W22" s="174" t="s">
+      <c r="W22" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="X22" s="175">
+      <c r="X22" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="Y22" s="173"/>
-      <c r="Z22" s="175">
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="80">
         <v>0.85763888888888884</v>
       </c>
-      <c r="AA22" s="173"/>
+      <c r="AA22" s="1"/>
       <c r="AB22" s="103" t="s">
         <v>106</v>
       </c>
@@ -5585,24 +5553,23 @@
       <c r="AM22" s="85" t="s">
         <v>122</v>
       </c>
-      <c r="AN22" s="174" t="s">
+      <c r="AN22" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="AO22" s="174" t="s">
+      <c r="AO22" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="AP22" s="175">
+      <c r="AP22" s="80">
         <v>0.5083333333333333</v>
       </c>
-      <c r="AQ22" s="173"/>
-      <c r="AR22" s="175">
+      <c r="AQ22" s="1"/>
+      <c r="AR22" s="80">
         <v>0.78472222222222221</v>
       </c>
-      <c r="AS22" s="173"/>
-      <c r="AT22" s="170" t="s">
+      <c r="AS22" s="1"/>
+      <c r="AT22" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="AU22" s="169"/>
       <c r="AV22" s="51"/>
     </row>
     <row r="23" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5633,7 +5600,7 @@
         <v>60</v>
       </c>
       <c r="R23" s="116"/>
-      <c r="S23" s="177"/>
+      <c r="S23" s="139"/>
       <c r="T23" s="81"/>
       <c r="U23" s="52"/>
       <c r="V23" s="67"/>
@@ -5660,38 +5627,36 @@
       <c r="AM23" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="AN23" s="178" t="s">
+      <c r="AN23" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="AO23" s="174" t="s">
+      <c r="AO23" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="AP23" s="175">
+      <c r="AP23" s="80">
         <v>0.78472222222222221</v>
       </c>
-      <c r="AQ23" s="173"/>
-      <c r="AR23" s="169"/>
-      <c r="AS23" s="173"/>
-      <c r="AT23" s="170" t="s">
+      <c r="AQ23" s="1"/>
+      <c r="AS23" s="1"/>
+      <c r="AT23" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="AU23" s="169"/>
       <c r="AV23" s="51"/>
     </row>
     <row r="24" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="144" t="s">
+      <c r="AG24" s="150" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="145"/>
+      <c r="AH24" s="151"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
       </c>
       <c r="AJ24" s="116"/>
-      <c r="AK24" s="177"/>
+      <c r="AK24" s="139"/>
       <c r="AL24" s="81"/>
       <c r="AM24" s="52"/>
-      <c r="AN24" s="179"/>
+      <c r="AN24" s="140"/>
       <c r="AO24" s="52"/>
       <c r="AP24" s="117"/>
       <c r="AQ24" s="117"/>

</xml_diff>

<commit_message>
Rw - Updates BeeHub - 20:30 PM
BeeHub Enabled

Transaction Placed For ShieldW
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B00B95AC-1FF1-4B26-B32B-A8E6F153A3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CBF66DF-CB01-40F2-9A95-D5D2E432374E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="140">
   <si>
     <t>UnSettled</t>
   </si>
@@ -447,6 +447,15 @@
   </si>
   <si>
     <t>Food- SS MgX</t>
+  </si>
+  <si>
+    <t>CNN Turk</t>
+  </si>
+  <si>
+    <t>18/12/2023</t>
+  </si>
+  <si>
+    <t>Al Jazeera E</t>
   </si>
 </sst>
 </file>
@@ -627,7 +636,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="43">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1173,11 +1182,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="191">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1492,7 +1512,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1584,6 +1603,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1869,7 +1936,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1886,9 +1953,9 @@
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="184" customWidth="1"/>
     <col min="15" max="15" width="4.85546875" style="1" customWidth="1"/>
-    <col min="16" max="16" width="9" customWidth="1"/>
+    <col min="16" max="16" width="9" style="1" customWidth="1"/>
     <col min="17" max="17" width="2.85546875" style="1" customWidth="1"/>
     <col min="18" max="18" width="11.140625" style="25" customWidth="1"/>
     <col min="19" max="19" width="5.140625" customWidth="1"/>
@@ -1903,9 +1970,9 @@
       <c r="B2" s="35">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="148">
+      <c r="C2" s="147">
         <f>B3+B4</f>
-        <v>1930</v>
+        <v>1800</v>
       </c>
       <c r="E2" s="101" t="s">
         <v>44</v>
@@ -1932,13 +1999,13 @@
       <c r="M2" s="127" t="s">
         <v>92</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="185" t="s">
         <v>68</v>
       </c>
       <c r="O2" s="38" t="s">
         <v>131</v>
       </c>
-      <c r="P2" s="91" t="s">
+      <c r="P2" s="190" t="s">
         <v>83</v>
       </c>
       <c r="Q2" s="102" t="s">
@@ -1953,21 +2020,21 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="146" t="s">
+      <c r="A3" s="145" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="35">
         <v>1500</v>
       </c>
-      <c r="C3" s="149"/>
+      <c r="C3" s="148"/>
       <c r="D3" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="147"/>
+      <c r="A4" s="146"/>
       <c r="B4" s="35">
-        <v>430</v>
+        <v>300</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>35</v>
@@ -1975,7 +2042,9 @@
       <c r="E4" s="135">
         <v>10</v>
       </c>
-      <c r="F4" s="39"/>
+      <c r="F4" s="39">
+        <v>10</v>
+      </c>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -1986,25 +2055,25 @@
         <v>89</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="K4" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="K4" s="175" t="s">
         <v>118</v>
       </c>
-      <c r="L4" s="30" t="s">
+      <c r="L4" s="177" t="s">
         <v>94</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="178" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="80">
-        <v>0.55625000000000002</v>
+      <c r="N4" s="186">
+        <v>0.83333333333333337</v>
       </c>
       <c r="P4" s="80">
-        <v>0.78472222222222221</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R4" s="25" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2014,7 +2083,9 @@
       <c r="E5" s="135">
         <v>10</v>
       </c>
-      <c r="F5" s="128"/>
+      <c r="F5" s="128">
+        <v>22</v>
+      </c>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2027,30 +2098,32 @@
       <c r="J5" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="K5" s="9" t="s">
+      <c r="K5" s="175" t="s">
         <v>119</v>
       </c>
-      <c r="L5" s="30" t="s">
-        <v>124</v>
-      </c>
-      <c r="M5" s="30" t="s">
+      <c r="L5" s="179" t="s">
+        <v>137</v>
+      </c>
+      <c r="M5" s="180" t="s">
         <v>86</v>
       </c>
-      <c r="N5" s="80">
-        <v>0.55625000000000002</v>
+      <c r="N5" s="186">
+        <v>0.83333333333333337</v>
       </c>
       <c r="P5" s="80">
-        <v>0.53472222222222221</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R5" s="25" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="135">
         <v>10</v>
       </c>
-      <c r="F6" s="129"/>
+      <c r="F6" s="129">
+        <v>20</v>
+      </c>
       <c r="G6" s="28" t="s">
         <v>135</v>
       </c>
@@ -2063,26 +2136,23 @@
       <c r="J6" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="175" t="s">
         <v>120</v>
       </c>
-      <c r="L6" s="30" t="s">
-        <v>133</v>
-      </c>
-      <c r="M6" s="30" t="s">
+      <c r="L6" s="181" t="s">
+        <v>21</v>
+      </c>
+      <c r="M6" s="180" t="s">
         <v>64</v>
       </c>
-      <c r="N6" s="80">
-        <v>0.55625000000000002</v>
-      </c>
-      <c r="O6" s="1" t="s">
-        <v>130</v>
+      <c r="N6" s="186">
+        <v>0.83333333333333337</v>
       </c>
       <c r="P6" s="80">
-        <v>0.5083333333333333</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R6" s="25" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2092,10 +2162,12 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="143">
+      <c r="E7" s="142">
         <v>3</v>
       </c>
-      <c r="F7" s="129"/>
+      <c r="F7" s="129">
+        <v>7</v>
+      </c>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2106,25 +2178,28 @@
         <v>105</v>
       </c>
       <c r="J7" s="39" t="s">
-        <v>125</v>
-      </c>
-      <c r="K7" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="K7" s="175" t="s">
         <v>91</v>
       </c>
-      <c r="L7" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="M7" s="30" t="s">
+      <c r="L7" s="181" t="s">
+        <v>85</v>
+      </c>
+      <c r="M7" s="180" t="s">
         <v>90</v>
       </c>
-      <c r="N7" s="80">
-        <v>0.56458333333333333</v>
+      <c r="N7" s="186">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>130</v>
       </c>
       <c r="P7" s="80">
-        <v>0.56458333333333333</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R7" s="25" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2144,16 +2219,16 @@
       <c r="J8" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="175" t="s">
         <v>121</v>
       </c>
-      <c r="L8" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="M8" s="30" t="s">
+      <c r="L8" s="181" t="s">
+        <v>123</v>
+      </c>
+      <c r="M8" s="180" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="80">
+      <c r="N8" s="186">
         <v>0.55625000000000002</v>
       </c>
       <c r="P8" s="80">
@@ -2169,7 +2244,7 @@
       </c>
       <c r="B9" s="8">
         <f>7000-C2</f>
-        <v>5070</v>
+        <v>5200</v>
       </c>
       <c r="E9" s="34">
         <v>25</v>
@@ -2178,42 +2253,42 @@
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="H9" s="122" t="s">
+      <c r="H9" s="189" t="s">
         <v>17</v>
       </c>
       <c r="I9" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="J9" s="34" t="s">
-        <v>21</v>
-      </c>
-      <c r="K9" s="9" t="s">
+      <c r="J9" s="34"/>
+      <c r="K9" s="175" t="s">
         <v>129</v>
       </c>
-      <c r="L9" s="30" t="s">
+      <c r="L9" s="181" t="s">
         <v>78</v>
       </c>
-      <c r="M9" s="30" t="s">
+      <c r="M9" s="180" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="80">
+      <c r="N9" s="186">
         <v>0.55625000000000002</v>
       </c>
       <c r="O9" s="1" t="s">
         <v>126</v>
       </c>
       <c r="P9" s="80">
-        <v>0.78472222222222221</v>
+        <v>0.55625000000000002</v>
       </c>
       <c r="R9" s="25" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="34">
         <v>70</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="39">
+        <v>70</v>
+      </c>
       <c r="G10" s="9" t="s">
         <v>81</v>
       </c>
@@ -2226,23 +2301,23 @@
       <c r="J10" s="39" t="s">
         <v>94</v>
       </c>
-      <c r="K10" s="85" t="s">
+      <c r="K10" s="176" t="s">
         <v>122</v>
       </c>
-      <c r="L10" s="30" t="s">
-        <v>22</v>
-      </c>
-      <c r="M10" s="30" t="s">
+      <c r="L10" s="181" t="s">
+        <v>124</v>
+      </c>
+      <c r="M10" s="180" t="s">
         <v>66</v>
       </c>
-      <c r="N10" s="80">
-        <v>0.55625000000000002</v>
+      <c r="N10" s="186">
+        <v>0.83333333333333337</v>
       </c>
       <c r="P10" s="80">
-        <v>0.78472222222222221</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R10" s="25" t="s">
-        <v>127</v>
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2253,10 +2328,12 @@
         <f>B9-B13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="143">
+      <c r="E11" s="142">
         <v>2</v>
       </c>
-      <c r="F11" s="39"/>
+      <c r="F11" s="39">
+        <v>1</v>
+      </c>
       <c r="G11" s="9" t="s">
         <v>128</v>
       </c>
@@ -2267,39 +2344,39 @@
         <v>116</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K11" s="175" t="s">
         <v>110</v>
       </c>
-      <c r="L11" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="M11" s="30" t="s">
+      <c r="L11" s="182" t="s">
+        <v>33</v>
+      </c>
+      <c r="M11" s="183" t="s">
         <v>66</v>
       </c>
-      <c r="N11" s="80">
-        <v>0.56458333333333333</v>
+      <c r="N11" s="186">
+        <v>0.83333333333333337</v>
       </c>
       <c r="P11" s="80">
-        <v>0.56458333333333333</v>
+        <v>0.83333333333333337</v>
       </c>
       <c r="R11" s="25" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="150" t="s">
+      <c r="E12" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="151"/>
+      <c r="F12" s="150"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>205</v>
+        <v>335</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
-      <c r="N12" s="24"/>
+      <c r="N12" s="187"/>
       <c r="O12" s="24"/>
     </row>
     <row r="13" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2308,15 +2385,15 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>5070</v>
+        <v>5200</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="121"/>
-      <c r="J13" s="144"/>
+      <c r="J13" s="143"/>
       <c r="L13"/>
       <c r="M13"/>
-      <c r="N13" s="145"/>
-      <c r="O13" s="145"/>
+      <c r="N13" s="188"/>
+      <c r="O13" s="144"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
@@ -2324,11 +2401,11 @@
       <c r="E14" s="24"/>
       <c r="F14" s="20"/>
       <c r="I14" s="121"/>
-      <c r="J14" s="144"/>
+      <c r="J14" s="143"/>
       <c r="L14"/>
       <c r="M14"/>
-      <c r="N14" s="145"/>
-      <c r="O14" s="145"/>
+      <c r="N14" s="188"/>
+      <c r="O14" s="144"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2342,12 +2419,12 @@
       <c r="E15" s="24"/>
       <c r="F15" s="20"/>
       <c r="I15" s="121"/>
-      <c r="J15" s="144"/>
+      <c r="J15" s="143"/>
       <c r="K15" s="121"/>
       <c r="L15"/>
       <c r="M15"/>
-      <c r="N15" s="145"/>
-      <c r="O15" s="145"/>
+      <c r="N15" s="188"/>
+      <c r="O15" s="144"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="25"/>
@@ -2366,8 +2443,8 @@
       <c r="I17" s="121"/>
       <c r="L17"/>
       <c r="M17"/>
-      <c r="N17" s="145"/>
-      <c r="O17" s="145"/>
+      <c r="N17" s="188"/>
+      <c r="O17" s="144"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2380,14 +2457,14 @@
       <c r="D18" s="25"/>
       <c r="E18" s="24"/>
       <c r="F18" s="20"/>
-      <c r="J18" s="144"/>
+      <c r="J18" s="143"/>
       <c r="L18"/>
       <c r="M18"/>
-      <c r="N18" s="145"/>
-      <c r="O18" s="145"/>
+      <c r="N18" s="188"/>
+      <c r="O18" s="144"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J19" s="144"/>
+      <c r="J19" s="143"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
@@ -2409,10 +2486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O24"/>
+  <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2435,18 +2512,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="159" t="s">
+      <c r="E1" s="158" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="160"/>
+      <c r="F1" s="159"/>
       <c r="G1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="159" t="s">
+      <c r="H1" s="158" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="161"/>
-      <c r="J1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="159"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2464,7 +2541,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="154">
+      <c r="B2" s="153">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2491,26 +2568,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="162">
+      <c r="K2" s="161">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="164">
+      <c r="L2" s="163">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="157">
+      <c r="M2" s="156">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J24)</f>
-        <v>5030</v>
+        <f>SUM(E2:J25)</f>
+        <v>5160</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="156"/>
+      <c r="B3" s="155"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2525,13 +2602,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="57"/>
-      <c r="K3" s="163"/>
-      <c r="L3" s="165"/>
-      <c r="M3" s="158"/>
+      <c r="K3" s="162"/>
+      <c r="L3" s="164"/>
+      <c r="M3" s="157"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="155"/>
+      <c r="B4" s="154"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2546,9 +2623,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="163"/>
-      <c r="L4" s="165"/>
-      <c r="M4" s="158"/>
+      <c r="K4" s="162"/>
+      <c r="L4" s="164"/>
+      <c r="M4" s="157"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2630,7 +2707,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="166">
+      <c r="B7" s="165">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2647,22 +2724,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="168">
+      <c r="K7" s="167">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="170">
+      <c r="L7" s="169">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="172">
+      <c r="M7" s="171">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="167"/>
+      <c r="B8" s="166"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2683,9 +2760,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="169"/>
-      <c r="L8" s="171"/>
-      <c r="M8" s="173"/>
+      <c r="K8" s="168"/>
+      <c r="L8" s="170"/>
+      <c r="M8" s="172"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2765,7 +2842,7 @@
       <c r="A11" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="166">
+      <c r="B11" s="165">
         <v>8</v>
       </c>
       <c r="C11" s="70"/>
@@ -2792,7 +2869,7 @@
       <c r="M11" s="72"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="167"/>
+      <c r="B12" s="166"/>
       <c r="C12" s="92">
         <v>483</v>
       </c>
@@ -2849,7 +2926,7 @@
       <c r="M13" s="84"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="166">
+      <c r="B14" s="165">
         <v>10</v>
       </c>
       <c r="C14" s="97"/>
@@ -2872,7 +2949,7 @@
       <c r="A15" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="167"/>
+      <c r="B15" s="166"/>
       <c r="C15" s="98"/>
       <c r="D15" s="84">
         <v>175</v>
@@ -2896,7 +2973,7 @@
       <c r="M15" s="93"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="154">
+      <c r="B16" s="153">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -2927,7 +3004,7 @@
       <c r="A17" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="156"/>
+      <c r="B17" s="155"/>
       <c r="C17" s="84"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
@@ -2945,7 +3022,7 @@
       <c r="M17" s="84"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="154">
+      <c r="B18" s="153">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -2974,7 +3051,7 @@
       <c r="A19" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="155"/>
+      <c r="B19" s="154"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3034,7 +3111,7 @@
       <c r="A21" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="152">
+      <c r="B21" s="151">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3062,7 +3139,7 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="153"/>
+      <c r="B22" s="152"/>
       <c r="C22" s="133"/>
       <c r="D22" s="134">
         <v>235</v>
@@ -3114,33 +3191,65 @@
       <c r="M23" s="72"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="132">
+      <c r="B24" s="147">
         <v>16</v>
       </c>
-      <c r="C24" s="58"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="59"/>
-      <c r="F24" s="59">
+      <c r="C24" s="173"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71">
         <v>75</v>
       </c>
-      <c r="G24" s="59">
+      <c r="G24" s="71">
         <v>70</v>
       </c>
-      <c r="H24" s="59">
+      <c r="H24" s="71">
         <v>30</v>
       </c>
-      <c r="I24" s="142">
+      <c r="I24" s="77">
         <v>5</v>
       </c>
-      <c r="J24" s="59">
+      <c r="J24" s="71">
         <v>25</v>
       </c>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="60"/>
+      <c r="K24" s="71"/>
+      <c r="L24" s="71"/>
+      <c r="M24" s="72"/>
+    </row>
+    <row r="25" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="B25" s="148"/>
+      <c r="C25" s="174"/>
+      <c r="D25" s="18">
+        <v>130</v>
+      </c>
+      <c r="E25" s="18">
+        <v>22</v>
+      </c>
+      <c r="F25" s="18">
+        <v>10</v>
+      </c>
+      <c r="G25" s="18">
+        <v>70</v>
+      </c>
+      <c r="H25" s="18">
+        <v>20</v>
+      </c>
+      <c r="I25" s="18">
+        <v>7</v>
+      </c>
+      <c r="J25" s="18">
+        <v>1</v>
+      </c>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="B24:B25"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B16:B17"/>
@@ -5644,10 +5753,10 @@
       <c r="AV23" s="51"/>
     </row>
     <row r="24" spans="1:48" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="150" t="s">
+      <c r="AG24" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="151"/>
+      <c r="AH24" s="150"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>

</xml_diff>

<commit_message>
Rw - Updates For France24F
Bridge Enabled For France24F
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9636D59-6D4A-4BCA-AF7F-37141B44ED8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0287313-BB55-4371-883E-1486D323B71F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="141">
   <si>
     <t>UnSettled</t>
   </si>
@@ -456,6 +456,9 @@
   </si>
   <si>
     <t>Al Jazeera E</t>
+  </si>
+  <si>
+    <t>France 24 F</t>
   </si>
 </sst>
 </file>
@@ -1587,46 +1590,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1936,7 +1939,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:O15"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,7 +2263,7 @@
         <v>115</v>
       </c>
       <c r="J9" s="34" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="K9" s="145" t="s">
         <v>129</v>
@@ -2278,7 +2281,7 @@
         <v>126</v>
       </c>
       <c r="P9" s="80">
-        <v>0.83333333333333337</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="R9" s="25" t="s">
         <v>134</v>
@@ -2514,18 +2517,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="176" t="s">
+      <c r="E1" s="169" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="177"/>
+      <c r="F1" s="170"/>
       <c r="G1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="176" t="s">
+      <c r="H1" s="169" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="178"/>
-      <c r="J1" s="177"/>
+      <c r="I1" s="171"/>
+      <c r="J1" s="170"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2543,7 +2546,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="171">
+      <c r="B2" s="172">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2570,15 +2573,15 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="179">
+      <c r="K2" s="175">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="181">
+      <c r="L2" s="177">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="174">
+      <c r="M2" s="181">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
@@ -2604,13 +2607,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="57"/>
-      <c r="K3" s="180"/>
-      <c r="L3" s="182"/>
-      <c r="M3" s="175"/>
+      <c r="K3" s="176"/>
+      <c r="L3" s="178"/>
+      <c r="M3" s="182"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="172"/>
+      <c r="B4" s="174"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2625,9 +2628,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="180"/>
-      <c r="L4" s="182"/>
-      <c r="M4" s="175"/>
+      <c r="K4" s="176"/>
+      <c r="L4" s="178"/>
+      <c r="M4" s="182"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2975,7 +2978,7 @@
       <c r="M15" s="93"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="171">
+      <c r="B16" s="172">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3024,7 +3027,7 @@
       <c r="M17" s="84"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="171">
+      <c r="B18" s="172">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3053,7 +3056,7 @@
       <c r="A19" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="172"/>
+      <c r="B19" s="174"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3113,7 +3116,7 @@
       <c r="A21" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="169">
+      <c r="B21" s="179">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3141,7 +3144,7 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="170"/>
+      <c r="B22" s="180"/>
       <c r="C22" s="133"/>
       <c r="D22" s="134">
         <v>235</v>
@@ -3251,11 +3254,6 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
@@ -3267,6 +3265,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Daily Usage - 6:55PM
Rw Daily Usage - 6:55PM
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4B6AD70-EC90-4CC0-AFE3-92CF73B0D4C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C4C135-84A9-4423-8C26-57B5D488B62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="141">
   <si>
     <t>UnSettled</t>
   </si>
@@ -1200,7 +1200,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="195">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1563,6 +1563,12 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1590,20 +1596,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1635,53 +1662,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1966,7 +1949,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,11 +1983,11 @@
       <c r="B2" s="35">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="165">
+      <c r="C2" s="167">
         <f>B3+B4</f>
-        <v>1800</v>
-      </c>
-      <c r="E2" s="201" t="s">
+        <v>1625</v>
+      </c>
+      <c r="E2" s="161" t="s">
         <v>44</v>
       </c>
       <c r="F2" s="105"/>
@@ -2050,31 +2033,29 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="163" t="s">
+      <c r="A3" s="165" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="35">
         <v>1500</v>
       </c>
-      <c r="C3" s="166"/>
+      <c r="C3" s="168"/>
       <c r="D3" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="164"/>
+      <c r="A4" s="166"/>
       <c r="B4" s="35">
-        <v>300</v>
+        <v>125</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="135">
-        <v>10</v>
-      </c>
-      <c r="F4" s="39">
-        <v>10</v>
-      </c>
+      <c r="E4" s="194">
+        <v>20</v>
+      </c>
+      <c r="F4" s="39"/>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -2091,15 +2072,15 @@
         <v>118</v>
       </c>
       <c r="L4" s="147" t="s">
-        <v>94</v>
+        <v>22</v>
       </c>
       <c r="M4" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="N4" s="156"/>
-      <c r="P4" s="80">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="N4" s="156">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="P4" s="80"/>
       <c r="R4" s="25" t="s">
         <v>134</v>
       </c>
@@ -2109,11 +2090,9 @@
         <v>-2</v>
       </c>
       <c r="E5" s="135">
-        <v>10</v>
-      </c>
-      <c r="F5" s="128">
-        <v>22</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F5" s="128"/>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2135,10 +2114,10 @@
       <c r="M5" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="N5" s="156"/>
-      <c r="P5" s="80">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="N5" s="156">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="P5" s="80"/>
       <c r="R5" s="25" t="s">
         <v>134</v>
       </c>
@@ -2147,9 +2126,7 @@
       <c r="E6" s="135">
         <v>10</v>
       </c>
-      <c r="F6" s="129">
-        <v>20</v>
-      </c>
+      <c r="F6" s="129"/>
       <c r="G6" s="28" t="s">
         <v>135</v>
       </c>
@@ -2165,16 +2142,16 @@
       <c r="K6" s="145" t="s">
         <v>120</v>
       </c>
-      <c r="L6" s="151" t="s">
-        <v>21</v>
+      <c r="L6" s="147" t="s">
+        <v>94</v>
       </c>
       <c r="M6" s="150" t="s">
         <v>64</v>
       </c>
-      <c r="N6" s="156"/>
-      <c r="P6" s="80">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="N6" s="156">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="P6" s="80"/>
       <c r="R6" s="25" t="s">
         <v>134</v>
       </c>
@@ -2187,11 +2164,9 @@
         <v>0</v>
       </c>
       <c r="E7" s="142">
-        <v>3</v>
-      </c>
-      <c r="F7" s="129">
-        <v>7</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F7" s="129"/>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2213,17 +2188,20 @@
       <c r="M7" s="150" t="s">
         <v>90</v>
       </c>
-      <c r="N7" s="156"/>
-      <c r="P7" s="80">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="N7" s="156">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="P7" s="80"/>
       <c r="R7" s="25" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="34">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="F8" s="39"/>
       <c r="G8" s="9" t="s">
@@ -2247,10 +2225,10 @@
       <c r="M8" s="150" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="156"/>
-      <c r="P8" s="80">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="N8" s="156">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="P8" s="80"/>
       <c r="R8" s="25" t="s">
         <v>134</v>
       </c>
@@ -2261,12 +2239,12 @@
       </c>
       <c r="B9" s="8">
         <f>7000-C2</f>
-        <v>5200</v>
-      </c>
-      <c r="E9" s="34">
-        <v>25</v>
-      </c>
-      <c r="F9" s="128"/>
+        <v>5375</v>
+      </c>
+      <c r="E9" s="34"/>
+      <c r="F9" s="128">
+        <v>5</v>
+      </c>
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
@@ -2288,20 +2266,18 @@
       <c r="M9" s="150" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="156"/>
-      <c r="P9" s="80">
-        <v>0.8666666666666667</v>
-      </c>
+      <c r="N9" s="156">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="P9" s="80"/>
       <c r="R9" s="25" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="34">
-        <v>70</v>
-      </c>
+      <c r="E10" s="34"/>
       <c r="F10" s="39">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="G10" s="9" t="s">
         <v>81</v>
@@ -2310,7 +2286,7 @@
         <v>17</v>
       </c>
       <c r="I10" s="85" t="s">
-        <v>114</v>
+        <v>32</v>
       </c>
       <c r="J10" s="39" t="s">
         <v>94</v>
@@ -2324,10 +2300,10 @@
       <c r="M10" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="N10" s="156"/>
-      <c r="P10" s="80">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="N10" s="156">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="P10" s="80"/>
       <c r="R10" s="25" t="s">
         <v>138</v>
       </c>
@@ -2341,11 +2317,9 @@
         <v>0</v>
       </c>
       <c r="E11" s="142">
-        <v>2</v>
-      </c>
-      <c r="F11" s="39">
-        <v>1</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F11" s="39"/>
       <c r="G11" s="9" t="s">
         <v>128</v>
       </c>
@@ -2367,22 +2341,25 @@
       <c r="M11" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="N11" s="156"/>
-      <c r="P11" s="80">
-        <v>0.83333333333333337</v>
-      </c>
+      <c r="N11" s="156">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="O11" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="P11" s="80"/>
       <c r="R11" s="25" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="167" t="s">
+      <c r="E12" s="169" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="168"/>
+      <c r="F12" s="170"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>335</v>
+        <v>175</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
@@ -2395,15 +2372,15 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>5200</v>
+        <v>5375</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="121"/>
-      <c r="J13" s="160"/>
+      <c r="J13" s="162"/>
       <c r="L13"/>
       <c r="M13"/>
-      <c r="N13" s="161"/>
-      <c r="O13" s="162"/>
+      <c r="N13" s="163"/>
+      <c r="O13" s="164"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
@@ -2411,11 +2388,11 @@
       <c r="E14" s="24"/>
       <c r="F14" s="20"/>
       <c r="I14" s="121"/>
-      <c r="J14" s="160"/>
+      <c r="J14" s="162"/>
       <c r="L14"/>
       <c r="M14"/>
-      <c r="N14" s="161"/>
-      <c r="O14" s="162"/>
+      <c r="N14" s="163"/>
+      <c r="O14" s="164"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2429,12 +2406,12 @@
       <c r="E15" s="24"/>
       <c r="F15" s="20"/>
       <c r="I15" s="121"/>
-      <c r="J15" s="160"/>
+      <c r="J15" s="162"/>
       <c r="K15" s="121"/>
       <c r="L15"/>
       <c r="M15"/>
-      <c r="N15" s="161"/>
-      <c r="O15" s="162"/>
+      <c r="N15" s="163"/>
+      <c r="O15" s="164"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="25"/>
@@ -2453,8 +2430,8 @@
       <c r="I17" s="121"/>
       <c r="L17"/>
       <c r="M17"/>
-      <c r="N17" s="161"/>
-      <c r="O17" s="162"/>
+      <c r="N17" s="163"/>
+      <c r="O17" s="164"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2467,14 +2444,14 @@
       <c r="D18" s="25"/>
       <c r="E18" s="24"/>
       <c r="F18" s="20"/>
-      <c r="J18" s="160"/>
+      <c r="J18" s="162"/>
       <c r="L18"/>
       <c r="M18"/>
-      <c r="N18" s="161"/>
-      <c r="O18" s="162"/>
+      <c r="N18" s="163"/>
+      <c r="O18" s="164"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J19" s="160"/>
+      <c r="J19" s="162"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
@@ -2496,7 +2473,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O26"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
@@ -2522,18 +2499,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="184" t="s">
+      <c r="E1" s="171" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="185"/>
+      <c r="F1" s="172"/>
       <c r="G1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="184" t="s">
+      <c r="H1" s="171" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="186"/>
-      <c r="J1" s="185"/>
+      <c r="I1" s="173"/>
+      <c r="J1" s="172"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2551,7 +2528,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="171">
+      <c r="B2" s="174">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2578,26 +2555,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="187">
+      <c r="K2" s="177">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="189">
+      <c r="L2" s="179">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="174">
+      <c r="M2" s="183">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J25)</f>
-        <v>5160</v>
+        <f>SUM(E2:J26)</f>
+        <v>5335</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="173"/>
+      <c r="B3" s="175"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2612,13 +2589,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="57"/>
-      <c r="K3" s="188"/>
-      <c r="L3" s="190"/>
-      <c r="M3" s="175"/>
+      <c r="K3" s="178"/>
+      <c r="L3" s="180"/>
+      <c r="M3" s="184"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="172"/>
+      <c r="B4" s="176"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2633,9 +2610,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="188"/>
-      <c r="L4" s="190"/>
-      <c r="M4" s="175"/>
+      <c r="K4" s="178"/>
+      <c r="L4" s="180"/>
+      <c r="M4" s="184"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2717,7 +2694,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="176">
+      <c r="B7" s="185">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2734,22 +2711,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="178">
+      <c r="K7" s="187">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="180">
+      <c r="L7" s="189">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="182">
+      <c r="M7" s="191">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="177"/>
+      <c r="B8" s="186"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2770,9 +2747,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="179"/>
-      <c r="L8" s="181"/>
-      <c r="M8" s="183"/>
+      <c r="K8" s="188"/>
+      <c r="L8" s="190"/>
+      <c r="M8" s="192"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2852,7 +2829,7 @@
       <c r="A11" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="176">
+      <c r="B11" s="185">
         <v>8</v>
       </c>
       <c r="C11" s="70"/>
@@ -2879,7 +2856,7 @@
       <c r="M11" s="72"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="177"/>
+      <c r="B12" s="186"/>
       <c r="C12" s="92">
         <v>483</v>
       </c>
@@ -2936,7 +2913,7 @@
       <c r="M13" s="84"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="176">
+      <c r="B14" s="185">
         <v>10</v>
       </c>
       <c r="C14" s="97"/>
@@ -2959,7 +2936,7 @@
       <c r="A15" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="177"/>
+      <c r="B15" s="186"/>
       <c r="C15" s="98"/>
       <c r="D15" s="84">
         <v>175</v>
@@ -2983,7 +2960,7 @@
       <c r="M15" s="93"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="171">
+      <c r="B16" s="174">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3014,7 +2991,7 @@
       <c r="A17" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="173"/>
+      <c r="B17" s="175"/>
       <c r="C17" s="84"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
@@ -3032,7 +3009,7 @@
       <c r="M17" s="84"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="171">
+      <c r="B18" s="174">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3061,7 +3038,7 @@
       <c r="A19" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="172"/>
+      <c r="B19" s="176"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3121,7 +3098,7 @@
       <c r="A21" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="169">
+      <c r="B21" s="181">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3149,7 +3126,7 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="170"/>
+      <c r="B22" s="182"/>
       <c r="C22" s="133"/>
       <c r="D22" s="134">
         <v>235</v>
@@ -3201,7 +3178,7 @@
       <c r="M23" s="72"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="165">
+      <c r="B24" s="167">
         <v>16</v>
       </c>
       <c r="C24" s="143"/>
@@ -3230,7 +3207,7 @@
       <c r="A25" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="166"/>
+      <c r="B25" s="168"/>
       <c r="C25" s="144"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -3257,13 +3234,36 @@
       <c r="L25" s="18"/>
       <c r="M25" s="18"/>
     </row>
+    <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="132">
+        <v>17</v>
+      </c>
+      <c r="C26" s="193"/>
+      <c r="D26" s="193"/>
+      <c r="E26" s="193">
+        <v>35</v>
+      </c>
+      <c r="F26" s="193">
+        <v>50</v>
+      </c>
+      <c r="G26" s="193">
+        <v>40</v>
+      </c>
+      <c r="H26" s="193">
+        <v>10</v>
+      </c>
+      <c r="I26" s="193">
+        <v>20</v>
+      </c>
+      <c r="J26" s="193">
+        <v>20</v>
+      </c>
+      <c r="K26" s="193"/>
+      <c r="L26" s="193"/>
+      <c r="M26" s="193"/>
+    </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
@@ -3275,6 +3275,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4968,20 +4973,17 @@
       <c r="AT15" s="25"/>
       <c r="AV15" s="51"/>
       <c r="AZ15" s="138"/>
-      <c r="BA15" s="191"/>
-      <c r="BB15" s="192"/>
-      <c r="BC15" s="193"/>
-      <c r="BD15" s="194"/>
-      <c r="BE15" s="191"/>
-      <c r="BF15" s="192"/>
-      <c r="BG15" s="195"/>
-      <c r="BH15" s="195"/>
-      <c r="BI15" s="197"/>
-      <c r="BJ15" s="195"/>
-      <c r="BK15" s="195"/>
-      <c r="BL15" s="195"/>
-      <c r="BM15" s="193"/>
-      <c r="BN15" s="192"/>
+      <c r="BA15" s="2"/>
+      <c r="BC15" s="25"/>
+      <c r="BD15" s="119"/>
+      <c r="BE15" s="2"/>
+      <c r="BG15" s="1"/>
+      <c r="BH15" s="1"/>
+      <c r="BI15" s="154"/>
+      <c r="BJ15" s="1"/>
+      <c r="BK15" s="1"/>
+      <c r="BL15" s="1"/>
+      <c r="BM15" s="25"/>
       <c r="BO15" s="51"/>
     </row>
     <row r="16" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5120,16 +5122,15 @@
       <c r="BH16" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="BI16" s="198"/>
-      <c r="BJ16" s="195"/>
-      <c r="BK16" s="199">
+      <c r="BI16" s="156"/>
+      <c r="BJ16" s="1"/>
+      <c r="BK16" s="80">
         <v>0.83333333333333337</v>
       </c>
-      <c r="BL16" s="195"/>
-      <c r="BM16" s="193" t="s">
+      <c r="BL16" s="1"/>
+      <c r="BM16" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="BN16" s="192"/>
       <c r="BO16" s="51"/>
     </row>
     <row r="17" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5270,16 +5271,15 @@
       <c r="BH17" s="150" t="s">
         <v>86</v>
       </c>
-      <c r="BI17" s="198"/>
-      <c r="BJ17" s="195"/>
-      <c r="BK17" s="199">
+      <c r="BI17" s="156"/>
+      <c r="BJ17" s="1"/>
+      <c r="BK17" s="80">
         <v>0.83333333333333337</v>
       </c>
-      <c r="BL17" s="195"/>
-      <c r="BM17" s="193" t="s">
+      <c r="BL17" s="1"/>
+      <c r="BM17" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="BN17" s="192"/>
       <c r="BO17" s="51"/>
     </row>
     <row r="18" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5399,7 +5399,7 @@
       <c r="BA18" s="129">
         <v>20</v>
       </c>
-      <c r="BB18" s="196" t="s">
+      <c r="BB18" s="28" t="s">
         <v>135</v>
       </c>
       <c r="BC18" s="122" t="s">
@@ -5420,16 +5420,15 @@
       <c r="BH18" s="150" t="s">
         <v>64</v>
       </c>
-      <c r="BI18" s="198"/>
-      <c r="BJ18" s="195"/>
-      <c r="BK18" s="199">
+      <c r="BI18" s="156"/>
+      <c r="BJ18" s="1"/>
+      <c r="BK18" s="80">
         <v>0.83333333333333337</v>
       </c>
-      <c r="BL18" s="195"/>
-      <c r="BM18" s="193" t="s">
+      <c r="BL18" s="1"/>
+      <c r="BM18" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="BN18" s="192"/>
       <c r="BO18" s="51"/>
     </row>
     <row r="19" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5566,16 +5565,15 @@
       <c r="BH19" s="150" t="s">
         <v>90</v>
       </c>
-      <c r="BI19" s="198"/>
-      <c r="BJ19" s="195"/>
-      <c r="BK19" s="199">
+      <c r="BI19" s="156"/>
+      <c r="BJ19" s="1"/>
+      <c r="BK19" s="80">
         <v>0.83333333333333337</v>
       </c>
-      <c r="BL19" s="195"/>
-      <c r="BM19" s="193" t="s">
+      <c r="BL19" s="1"/>
+      <c r="BM19" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="BN19" s="192"/>
       <c r="BO19" s="51"/>
     </row>
     <row r="20" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5710,16 +5708,15 @@
       <c r="BH20" s="150" t="s">
         <v>69</v>
       </c>
-      <c r="BI20" s="198"/>
-      <c r="BJ20" s="195"/>
-      <c r="BK20" s="199">
+      <c r="BI20" s="156"/>
+      <c r="BJ20" s="1"/>
+      <c r="BK20" s="80">
         <v>0.83333333333333337</v>
       </c>
-      <c r="BL20" s="195"/>
-      <c r="BM20" s="193" t="s">
+      <c r="BL20" s="1"/>
+      <c r="BM20" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="BN20" s="192"/>
       <c r="BO20" s="51"/>
     </row>
     <row r="21" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5856,16 +5853,15 @@
       <c r="BH21" s="150" t="s">
         <v>64</v>
       </c>
-      <c r="BI21" s="198"/>
-      <c r="BJ21" s="195"/>
-      <c r="BK21" s="199">
+      <c r="BI21" s="156"/>
+      <c r="BJ21" s="1"/>
+      <c r="BK21" s="80">
         <v>0.8666666666666667</v>
       </c>
-      <c r="BL21" s="195"/>
-      <c r="BM21" s="193" t="s">
+      <c r="BL21" s="1"/>
+      <c r="BM21" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="BN21" s="192"/>
       <c r="BO21" s="51"/>
     </row>
     <row r="22" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6002,16 +5998,15 @@
       <c r="BH22" s="150" t="s">
         <v>66</v>
       </c>
-      <c r="BI22" s="198"/>
-      <c r="BJ22" s="195"/>
-      <c r="BK22" s="199">
+      <c r="BI22" s="156"/>
+      <c r="BJ22" s="1"/>
+      <c r="BK22" s="80">
         <v>0.83333333333333337</v>
       </c>
-      <c r="BL22" s="195"/>
-      <c r="BM22" s="193" t="s">
+      <c r="BL22" s="1"/>
+      <c r="BM22" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="BN22" s="192"/>
       <c r="BO22" s="51"/>
     </row>
     <row r="23" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6115,23 +6110,22 @@
       <c r="BH23" s="153" t="s">
         <v>66</v>
       </c>
-      <c r="BI23" s="198"/>
-      <c r="BJ23" s="195"/>
-      <c r="BK23" s="199">
+      <c r="BI23" s="156"/>
+      <c r="BJ23" s="1"/>
+      <c r="BK23" s="80">
         <v>0.83333333333333337</v>
       </c>
-      <c r="BL23" s="195"/>
-      <c r="BM23" s="193" t="s">
+      <c r="BL23" s="1"/>
+      <c r="BM23" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="BN23" s="192"/>
       <c r="BO23" s="51"/>
     </row>
     <row r="24" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="167" t="s">
+      <c r="AG24" s="169" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="168"/>
+      <c r="AH24" s="170"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -6151,10 +6145,10 @@
       <c r="AV24" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="167" t="s">
+      <c r="AZ24" s="169" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="168"/>
+      <c r="BA24" s="170"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -6165,7 +6159,7 @@
       <c r="BF24" s="52"/>
       <c r="BG24" s="140"/>
       <c r="BH24" s="52"/>
-      <c r="BI24" s="200"/>
+      <c r="BI24" s="160"/>
       <c r="BJ24" s="117"/>
       <c r="BK24" s="67"/>
       <c r="BL24" s="67"/>

</xml_diff>

<commit_message>
Rw Usage Sync 9:39 PM
Rw Usage Sync _18122023
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{246F74FB-9C40-473C-A4CB-E0C704AF7C3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AD4994D-A222-49ED-8F24-5D6AF60F323D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="717" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="143">
   <si>
     <t>UnSettled</t>
   </si>
@@ -462,6 +462,9 @@
   </si>
   <si>
     <t>19/12/2023</t>
+  </si>
+  <si>
+    <t>Rw- Mumbai</t>
   </si>
 </sst>
 </file>
@@ -642,7 +645,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1199,11 +1202,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="197">
+  <cellXfs count="208">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1603,20 +1617,41 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1648,29 +1683,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1954,7 +1995,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1967,7 +2008,7 @@
     <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.28515625" style="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="119" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.42578125" style="1" customWidth="1"/>
     <col min="13" max="13" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -1990,7 +2031,7 @@
       </c>
       <c r="C2" s="169">
         <f>B3+B4</f>
-        <v>1525</v>
+        <v>1505</v>
       </c>
       <c r="E2" s="161" t="s">
         <v>44</v>
@@ -2034,7 +2075,7 @@
       </c>
       <c r="T2" s="100">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
+        <v>45278</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2052,17 +2093,15 @@
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="168"/>
       <c r="B4" s="35">
-        <v>25</v>
+        <v>5</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>35</v>
       </c>
       <c r="E4" s="163">
-        <v>20</v>
-      </c>
-      <c r="F4" s="39">
-        <v>5</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F4" s="39"/>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -2073,13 +2112,13 @@
         <v>89</v>
       </c>
       <c r="J4" s="39" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="K4" s="145" t="s">
-        <v>118</v>
+        <v>142</v>
       </c>
       <c r="L4" s="147" t="s">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="M4" s="148" t="s">
         <v>30</v>
@@ -2099,11 +2138,9 @@
         <v>-2</v>
       </c>
       <c r="E5" s="135">
-        <v>40</v>
-      </c>
-      <c r="F5" s="128">
         <v>10</v>
       </c>
+      <c r="F5" s="128"/>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2136,12 +2173,8 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="135">
-        <v>10</v>
-      </c>
-      <c r="F6" s="129">
-        <v>5</v>
-      </c>
+      <c r="E6" s="135"/>
+      <c r="F6" s="129"/>
       <c r="G6" s="28" t="s">
         <v>135</v>
       </c>
@@ -2154,9 +2187,7 @@
       <c r="J6" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="145" t="s">
-        <v>120</v>
-      </c>
+      <c r="K6" s="145"/>
       <c r="L6" s="147" t="s">
         <v>94</v>
       </c>
@@ -2180,12 +2211,8 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="142">
-        <v>10</v>
-      </c>
-      <c r="F7" s="129">
-        <v>7</v>
-      </c>
+      <c r="E7" s="142"/>
+      <c r="F7" s="129"/>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2221,9 +2248,7 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="34">
-        <v>50</v>
-      </c>
+      <c r="E8" s="34"/>
       <c r="F8" s="39"/>
       <c r="G8" s="9" t="s">
         <v>72</v>
@@ -2260,12 +2285,10 @@
       </c>
       <c r="B9" s="8">
         <f>7000-C2</f>
-        <v>5475</v>
+        <v>5495</v>
       </c>
       <c r="E9" s="34"/>
-      <c r="F9" s="128">
-        <v>5</v>
-      </c>
+      <c r="F9" s="128"/>
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
@@ -2296,12 +2319,8 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="34">
-        <v>70</v>
-      </c>
-      <c r="F10" s="39">
-        <v>30</v>
-      </c>
+      <c r="E10" s="34"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="9" t="s">
         <v>81</v>
       </c>
@@ -2339,12 +2358,8 @@
         <f>B9-B13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="142">
-        <v>10</v>
-      </c>
-      <c r="F11" s="39">
-        <v>3</v>
-      </c>
+      <c r="E11" s="142"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="9" t="s">
         <v>128</v>
       </c>
@@ -2386,7 +2401,7 @@
       <c r="F12" s="172"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>275</v>
+        <v>20</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
@@ -2399,7 +2414,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>5475</v>
+        <v>5495</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="121"/>
@@ -2500,10 +2515,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2526,18 +2541,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="188" t="s">
+      <c r="E1" s="173" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="189"/>
+      <c r="F1" s="174"/>
       <c r="G1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="188" t="s">
+      <c r="H1" s="173" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="190"/>
-      <c r="J1" s="189"/>
+      <c r="I1" s="175"/>
+      <c r="J1" s="174"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2555,7 +2570,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="175">
+      <c r="B2" s="176">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2582,21 +2597,21 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="191">
+      <c r="K2" s="179">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="193">
+      <c r="L2" s="181">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="178">
+      <c r="M2" s="185">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J27)</f>
-        <v>5435</v>
+        <f>SUM(E2:J28)</f>
+        <v>5455</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -2616,13 +2631,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="57"/>
-      <c r="K3" s="192"/>
-      <c r="L3" s="194"/>
-      <c r="M3" s="179"/>
+      <c r="K3" s="180"/>
+      <c r="L3" s="182"/>
+      <c r="M3" s="186"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="176"/>
+      <c r="B4" s="178"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2637,9 +2652,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="192"/>
-      <c r="L4" s="194"/>
-      <c r="M4" s="179"/>
+      <c r="K4" s="180"/>
+      <c r="L4" s="182"/>
+      <c r="M4" s="186"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2721,7 +2736,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="180">
+      <c r="B7" s="187">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2738,22 +2753,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="182">
+      <c r="K7" s="189">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="184">
+      <c r="L7" s="191">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="186">
+      <c r="M7" s="193">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="181"/>
+      <c r="B8" s="188"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2774,9 +2789,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="183"/>
-      <c r="L8" s="185"/>
-      <c r="M8" s="187"/>
+      <c r="K8" s="190"/>
+      <c r="L8" s="192"/>
+      <c r="M8" s="194"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2856,7 +2871,7 @@
       <c r="A11" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="180">
+      <c r="B11" s="187">
         <v>8</v>
       </c>
       <c r="C11" s="70"/>
@@ -2883,7 +2898,7 @@
       <c r="M11" s="72"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="181"/>
+      <c r="B12" s="188"/>
       <c r="C12" s="92">
         <v>483</v>
       </c>
@@ -2940,7 +2955,7 @@
       <c r="M13" s="84"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="180">
+      <c r="B14" s="187">
         <v>10</v>
       </c>
       <c r="C14" s="97"/>
@@ -2963,7 +2978,7 @@
       <c r="A15" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="181"/>
+      <c r="B15" s="188"/>
       <c r="C15" s="98"/>
       <c r="D15" s="84">
         <v>175</v>
@@ -2987,7 +3002,7 @@
       <c r="M15" s="93"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="175">
+      <c r="B16" s="176">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3036,7 +3051,7 @@
       <c r="M17" s="84"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="175">
+      <c r="B18" s="176">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3065,7 +3080,7 @@
       <c r="A19" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="176"/>
+      <c r="B19" s="178"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3125,7 +3140,7 @@
       <c r="A21" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="173">
+      <c r="B21" s="183">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3153,7 +3168,7 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="174"/>
+      <c r="B22" s="184"/>
       <c r="C22" s="133"/>
       <c r="D22" s="134">
         <v>235</v>
@@ -3262,10 +3277,10 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="132">
-        <v>17</v>
-      </c>
-      <c r="C26" s="162"/>
+      <c r="B26" s="169">
+        <v>17</v>
+      </c>
+      <c r="C26" s="204"/>
       <c r="D26" s="162"/>
       <c r="E26" s="162">
         <v>35</v>
@@ -3289,40 +3304,63 @@
       <c r="L26" s="162"/>
       <c r="M26" s="162"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C27" s="18"/>
-      <c r="D27" s="195">
+    <row r="27" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="205"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="134">
         <v>100</v>
       </c>
-      <c r="E27" s="196">
+      <c r="E27" s="84">
         <v>5</v>
       </c>
-      <c r="F27" s="196">
+      <c r="F27" s="84">
         <v>3</v>
       </c>
-      <c r="G27" s="196">
+      <c r="G27" s="84">
         <v>70</v>
       </c>
-      <c r="H27" s="196">
+      <c r="H27" s="84">
         <v>10</v>
       </c>
-      <c r="I27" s="18">
+      <c r="I27" s="84">
         <v>7</v>
       </c>
-      <c r="J27" s="196">
+      <c r="J27" s="84">
         <v>5</v>
       </c>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
-      <c r="M27" s="18"/>
+      <c r="K27" s="84"/>
+      <c r="L27" s="84"/>
+      <c r="M27" s="84"/>
+    </row>
+    <row r="28" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="86" t="s">
+        <v>1</v>
+      </c>
+      <c r="B28" s="206">
+        <v>18</v>
+      </c>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="207">
+        <v>10</v>
+      </c>
+      <c r="I28" s="207">
+        <v>10</v>
+      </c>
+      <c r="J28" s="59"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
+  <mergeCells count="17">
+    <mergeCell ref="B26:B27"/>
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
@@ -3334,6 +3372,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3341,10 +3384,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EF39B9-450C-4C51-9807-7AFD5CC29C14}">
-  <dimension ref="A1:BV24"/>
+  <dimension ref="A1:CG24"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView topLeftCell="BN6" workbookViewId="0">
+      <selection activeCell="BP15" sqref="BP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3367,7 +3410,7 @@
     <col min="70" max="70" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" s="44"/>
       <c r="C1" s="45"/>
       <c r="D1" s="45"/>
@@ -3534,7 +3577,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="26">
         <v>27</v>
       </c>
@@ -3606,7 +3649,7 @@
       <c r="BU2" s="1"/>
       <c r="BV2" s="49"/>
     </row>
-    <row r="3" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="26">
         <v>20</v>
       </c>
@@ -3761,7 +3804,7 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="4" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26">
         <v>400</v>
       </c>
@@ -3934,7 +3977,7 @@
         <v>0.48888888888888887</v>
       </c>
     </row>
-    <row r="5" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="26">
         <v>200</v>
       </c>
@@ -4087,7 +4130,7 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="6" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="26">
         <v>40</v>
       </c>
@@ -4235,7 +4278,7 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="7" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="26">
         <v>130</v>
       </c>
@@ -4401,7 +4444,7 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="8" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="50"/>
       <c r="C8" s="9">
         <f>SUM(B3:B7)</f>
@@ -4547,7 +4590,7 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="9" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="50"/>
       <c r="D9" s="8"/>
       <c r="I9" s="49"/>
@@ -4681,7 +4724,7 @@
         <v>0.51388888888888895</v>
       </c>
     </row>
-    <row r="10" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9" t="s">
         <v>4</v>
       </c>
@@ -4798,12 +4841,12 @@
       <c r="BU10" s="67"/>
       <c r="BV10" s="69"/>
     </row>
-    <row r="11" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="50"/>
       <c r="I11" s="51"/>
       <c r="AS11" s="1"/>
     </row>
-    <row r="12" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="37">
         <v>45028</v>
       </c>
@@ -4815,8 +4858,8 @@
       <c r="H12" s="52"/>
       <c r="I12" s="53"/>
     </row>
-    <row r="13" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="14" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="14" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="110"/>
       <c r="B14" s="101" t="s">
         <v>44</v>
@@ -4894,7 +4937,7 @@
       </c>
       <c r="AC14" s="100">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
+        <v>45278</v>
       </c>
       <c r="AG14" s="101" t="s">
         <v>44</v>
@@ -4939,7 +4982,7 @@
       <c r="AU14" s="45"/>
       <c r="AV14" s="100">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
+        <v>45278</v>
       </c>
       <c r="AZ14" s="101" t="s">
         <v>44</v>
@@ -4984,10 +5027,55 @@
       <c r="BN14" s="45"/>
       <c r="BO14" s="100">
         <f ca="1">TODAY()</f>
-        <v>45277</v>
-      </c>
-    </row>
-    <row r="15" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45278</v>
+      </c>
+      <c r="BR14" s="161" t="s">
+        <v>44</v>
+      </c>
+      <c r="BS14" s="105"/>
+      <c r="BT14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="BU14" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="BV14" s="85" t="s">
+        <v>41</v>
+      </c>
+      <c r="BW14" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="BX14" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BY14" s="127" t="s">
+        <v>38</v>
+      </c>
+      <c r="BZ14" s="127" t="s">
+        <v>92</v>
+      </c>
+      <c r="CA14" s="155" t="s">
+        <v>68</v>
+      </c>
+      <c r="CB14" s="38" t="s">
+        <v>131</v>
+      </c>
+      <c r="CC14" s="159" t="s">
+        <v>83</v>
+      </c>
+      <c r="CD14" s="102" t="s">
+        <v>36</v>
+      </c>
+      <c r="CE14" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="CF14" s="45"/>
+      <c r="CG14" s="100">
+        <f ca="1">TODAY()</f>
+        <v>45278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="105" t="s">
         <v>36</v>
       </c>
@@ -5039,8 +5127,24 @@
       <c r="BL15" s="1"/>
       <c r="BM15" s="25"/>
       <c r="BO15" s="51"/>
-    </row>
-    <row r="16" spans="1:74" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR15" s="138"/>
+      <c r="BS15" s="195"/>
+      <c r="BT15" s="196"/>
+      <c r="BU15" s="197"/>
+      <c r="BV15" s="198"/>
+      <c r="BW15" s="195"/>
+      <c r="BX15" s="196"/>
+      <c r="BY15" s="199"/>
+      <c r="BZ15" s="199"/>
+      <c r="CA15" s="200"/>
+      <c r="CB15" s="199"/>
+      <c r="CC15" s="199"/>
+      <c r="CD15" s="199"/>
+      <c r="CE15" s="197"/>
+      <c r="CF15" s="196"/>
+      <c r="CG15" s="51"/>
+    </row>
+    <row r="16" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="112"/>
       <c r="B16" s="38">
         <v>10</v>
@@ -5186,8 +5290,48 @@
         <v>134</v>
       </c>
       <c r="BO16" s="51"/>
-    </row>
-    <row r="17" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR16" s="163">
+        <v>20</v>
+      </c>
+      <c r="BS16" s="39">
+        <v>5</v>
+      </c>
+      <c r="BT16" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="BU16" s="109" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV16" s="120" t="s">
+        <v>89</v>
+      </c>
+      <c r="BW16" s="39" t="s">
+        <v>139</v>
+      </c>
+      <c r="BX16" s="145" t="s">
+        <v>118</v>
+      </c>
+      <c r="BY16" s="147" t="s">
+        <v>22</v>
+      </c>
+      <c r="BZ16" s="148" t="s">
+        <v>30</v>
+      </c>
+      <c r="CA16" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CB16" s="199"/>
+      <c r="CC16" s="201">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="CD16" s="199"/>
+      <c r="CE16" s="197" t="s">
+        <v>138</v>
+      </c>
+      <c r="CF16" s="196"/>
+      <c r="CG16" s="51"/>
+    </row>
+    <row r="17" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="107">
         <v>-2</v>
       </c>
@@ -5335,8 +5479,48 @@
         <v>134</v>
       </c>
       <c r="BO17" s="51"/>
-    </row>
-    <row r="18" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR17" s="135">
+        <v>40</v>
+      </c>
+      <c r="BS17" s="128">
+        <v>10</v>
+      </c>
+      <c r="BT17" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="BU17" s="109" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV17" s="85" t="s">
+        <v>113</v>
+      </c>
+      <c r="BW17" s="39" t="s">
+        <v>85</v>
+      </c>
+      <c r="BX17" s="145" t="s">
+        <v>119</v>
+      </c>
+      <c r="BY17" s="149" t="s">
+        <v>137</v>
+      </c>
+      <c r="BZ17" s="150" t="s">
+        <v>86</v>
+      </c>
+      <c r="CA17" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CB17" s="199"/>
+      <c r="CC17" s="201">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="CD17" s="199"/>
+      <c r="CE17" s="197" t="s">
+        <v>138</v>
+      </c>
+      <c r="CF17" s="196"/>
+      <c r="CG17" s="51"/>
+    </row>
+    <row r="18" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="112"/>
       <c r="B18" s="38">
         <v>20</v>
@@ -5484,8 +5668,48 @@
         <v>134</v>
       </c>
       <c r="BO18" s="51"/>
-    </row>
-    <row r="19" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR18" s="135">
+        <v>10</v>
+      </c>
+      <c r="BS18" s="129">
+        <v>5</v>
+      </c>
+      <c r="BT18" s="202" t="s">
+        <v>135</v>
+      </c>
+      <c r="BU18" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV18" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="BW18" s="39" t="s">
+        <v>102</v>
+      </c>
+      <c r="BX18" s="145" t="s">
+        <v>120</v>
+      </c>
+      <c r="BY18" s="147" t="s">
+        <v>94</v>
+      </c>
+      <c r="BZ18" s="150" t="s">
+        <v>64</v>
+      </c>
+      <c r="CA18" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CB18" s="199"/>
+      <c r="CC18" s="201">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="CD18" s="199"/>
+      <c r="CE18" s="197" t="s">
+        <v>138</v>
+      </c>
+      <c r="CF18" s="196"/>
+      <c r="CG18" s="51"/>
+    </row>
+    <row r="19" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="112"/>
       <c r="B19" s="38">
         <v>10</v>
@@ -5629,8 +5853,50 @@
         <v>134</v>
       </c>
       <c r="BO19" s="51"/>
-    </row>
-    <row r="20" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR19" s="142">
+        <v>10</v>
+      </c>
+      <c r="BS19" s="129">
+        <v>7</v>
+      </c>
+      <c r="BT19" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="BU19" s="126" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV19" s="85" t="s">
+        <v>105</v>
+      </c>
+      <c r="BW19" s="39" t="s">
+        <v>137</v>
+      </c>
+      <c r="BX19" s="145" t="s">
+        <v>91</v>
+      </c>
+      <c r="BY19" s="151" t="s">
+        <v>85</v>
+      </c>
+      <c r="BZ19" s="150" t="s">
+        <v>90</v>
+      </c>
+      <c r="CA19" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CB19" s="199" t="s">
+        <v>130</v>
+      </c>
+      <c r="CC19" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CD19" s="199"/>
+      <c r="CE19" s="197" t="s">
+        <v>138</v>
+      </c>
+      <c r="CF19" s="196"/>
+      <c r="CG19" s="51"/>
+    </row>
+    <row r="20" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="112"/>
       <c r="B20" s="38">
         <v>25</v>
@@ -5772,8 +6038,44 @@
         <v>134</v>
       </c>
       <c r="BO20" s="51"/>
-    </row>
-    <row r="21" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR20" s="34">
+        <v>50</v>
+      </c>
+      <c r="BS20" s="39"/>
+      <c r="BT20" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="BU20" s="109" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV20" s="85" t="s">
+        <v>70</v>
+      </c>
+      <c r="BW20" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="BX20" s="145" t="s">
+        <v>121</v>
+      </c>
+      <c r="BY20" s="151" t="s">
+        <v>123</v>
+      </c>
+      <c r="BZ20" s="150" t="s">
+        <v>69</v>
+      </c>
+      <c r="CA20" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CB20" s="199"/>
+      <c r="CC20" s="201"/>
+      <c r="CD20" s="199"/>
+      <c r="CE20" s="197" t="s">
+        <v>141</v>
+      </c>
+      <c r="CF20" s="196"/>
+      <c r="CG20" s="51"/>
+    </row>
+    <row r="21" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="112"/>
       <c r="B21" s="38">
         <v>95</v>
@@ -5917,8 +6219,44 @@
         <v>134</v>
       </c>
       <c r="BO21" s="51"/>
-    </row>
-    <row r="22" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR21" s="34"/>
+      <c r="BS21" s="128">
+        <v>5</v>
+      </c>
+      <c r="BT21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU21" s="158" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV21" s="85" t="s">
+        <v>115</v>
+      </c>
+      <c r="BW21" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="BX21" s="145" t="s">
+        <v>129</v>
+      </c>
+      <c r="BY21" s="151" t="s">
+        <v>78</v>
+      </c>
+      <c r="BZ21" s="150" t="s">
+        <v>64</v>
+      </c>
+      <c r="CA21" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CB21" s="199"/>
+      <c r="CC21" s="203"/>
+      <c r="CD21" s="199"/>
+      <c r="CE21" s="197" t="s">
+        <v>141</v>
+      </c>
+      <c r="CF21" s="196"/>
+      <c r="CG21" s="51"/>
+    </row>
+    <row r="22" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="112"/>
       <c r="B22" s="38">
         <v>70</v>
@@ -6062,8 +6400,46 @@
         <v>138</v>
       </c>
       <c r="BO22" s="51"/>
-    </row>
-    <row r="23" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR22" s="34">
+        <v>70</v>
+      </c>
+      <c r="BS22" s="39">
+        <v>30</v>
+      </c>
+      <c r="BT22" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="BU22" s="124" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV22" s="85" t="s">
+        <v>32</v>
+      </c>
+      <c r="BW22" s="39" t="s">
+        <v>94</v>
+      </c>
+      <c r="BX22" s="146" t="s">
+        <v>122</v>
+      </c>
+      <c r="BY22" s="151" t="s">
+        <v>124</v>
+      </c>
+      <c r="BZ22" s="150" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA22" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CB22" s="199"/>
+      <c r="CC22" s="203"/>
+      <c r="CD22" s="199"/>
+      <c r="CE22" s="197" t="s">
+        <v>141</v>
+      </c>
+      <c r="CF22" s="196"/>
+      <c r="CG22" s="51"/>
+    </row>
+    <row r="23" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="115"/>
       <c r="B23" s="34" t="s">
         <v>4</v>
@@ -6174,8 +6550,50 @@
         <v>134</v>
       </c>
       <c r="BO23" s="51"/>
-    </row>
-    <row r="24" spans="1:67" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="BR23" s="142">
+        <v>10</v>
+      </c>
+      <c r="BS23" s="39">
+        <v>3</v>
+      </c>
+      <c r="BT23" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="BU23" s="109" t="s">
+        <v>17</v>
+      </c>
+      <c r="BV23" s="120" t="s">
+        <v>116</v>
+      </c>
+      <c r="BW23" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="BX23" s="145" t="s">
+        <v>110</v>
+      </c>
+      <c r="BY23" s="152" t="s">
+        <v>33</v>
+      </c>
+      <c r="BZ23" s="153" t="s">
+        <v>66</v>
+      </c>
+      <c r="CA23" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CB23" s="199" t="s">
+        <v>126</v>
+      </c>
+      <c r="CC23" s="201">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="CD23" s="199"/>
+      <c r="CE23" s="197" t="s">
+        <v>138</v>
+      </c>
+      <c r="CF23" s="196"/>
+      <c r="CG23" s="51"/>
+    </row>
+    <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="AG24" s="171" t="s">
         <v>4</v>
       </c>
@@ -6222,11 +6640,35 @@
       <c r="BO24" s="53" t="s">
         <v>127</v>
       </c>
+      <c r="BR24" s="171" t="s">
+        <v>4</v>
+      </c>
+      <c r="BS24" s="172"/>
+      <c r="BT24" s="9">
+        <f>SUM(BR16:BS23)</f>
+        <v>275</v>
+      </c>
+      <c r="BU24" s="116"/>
+      <c r="BV24" s="139"/>
+      <c r="BW24" s="81"/>
+      <c r="BX24" s="52"/>
+      <c r="BY24" s="140"/>
+      <c r="BZ24" s="52"/>
+      <c r="CA24" s="160"/>
+      <c r="CB24" s="117"/>
+      <c r="CC24" s="67"/>
+      <c r="CD24" s="67"/>
+      <c r="CE24" s="116"/>
+      <c r="CF24" s="52"/>
+      <c r="CG24" s="104" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
+    <mergeCell ref="BR24:BS24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Sync_18122023 7:31PM
Rw Usage Sync_18122023
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723738BE-15BD-4320-AE73-4C8C0CF45C88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05727EAB-9323-4D06-8219-F1B6DFB057F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="146">
   <si>
     <t>UnSettled</t>
   </si>
@@ -465,6 +465,15 @@
   </si>
   <si>
     <t>Rw- Mumbai</t>
+  </si>
+  <si>
+    <t>TBS News</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>20/12/2023</t>
   </si>
 </sst>
 </file>
@@ -1217,7 +1226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1591,9 +1600,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1621,23 +1627,35 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1669,27 +1687,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1973,7 +1983,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2007,9 +2017,9 @@
       <c r="B2" s="35">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="171">
+      <c r="C2" s="170">
         <f>B3+B4</f>
-        <v>1505</v>
+        <v>1013</v>
       </c>
       <c r="E2" s="161" t="s">
         <v>44</v>
@@ -2057,21 +2067,21 @@
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="169" t="s">
+      <c r="A3" s="168" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="35">
-        <v>1500</v>
-      </c>
-      <c r="C3" s="172"/>
+        <v>500</v>
+      </c>
+      <c r="C3" s="171"/>
       <c r="D3" s="36" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="170"/>
+      <c r="A4" s="169"/>
       <c r="B4" s="35">
-        <v>5</v>
+        <v>513</v>
       </c>
       <c r="C4" s="34" t="s">
         <v>35</v>
@@ -2079,7 +2089,9 @@
       <c r="E4" s="163">
         <v>10</v>
       </c>
-      <c r="F4" s="39"/>
+      <c r="F4" s="39">
+        <v>42</v>
+      </c>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -2102,7 +2114,7 @@
         <v>30</v>
       </c>
       <c r="N4" s="156">
-        <v>0.41666666666666669</v>
+        <v>0.80972222222222223</v>
       </c>
       <c r="P4" s="156">
         <v>0.87152777777777779</v>
@@ -2118,7 +2130,9 @@
       <c r="E5" s="135">
         <v>10</v>
       </c>
-      <c r="F5" s="128"/>
+      <c r="F5" s="128">
+        <v>20</v>
+      </c>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2141,7 +2155,7 @@
         <v>86</v>
       </c>
       <c r="N5" s="156">
-        <v>0.41666666666666669</v>
+        <v>0.80972222222222223</v>
       </c>
       <c r="P5" s="156">
         <v>0.87152777777777779</v>
@@ -2151,8 +2165,12 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="135"/>
-      <c r="F6" s="129"/>
+      <c r="E6" s="135">
+        <v>222</v>
+      </c>
+      <c r="F6" s="129">
+        <v>10</v>
+      </c>
       <c r="G6" s="28" t="s">
         <v>135</v>
       </c>
@@ -2165,7 +2183,9 @@
       <c r="J6" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="K6" s="145"/>
+      <c r="K6" s="145" t="s">
+        <v>120</v>
+      </c>
       <c r="L6" s="147" t="s">
         <v>94</v>
       </c>
@@ -2173,7 +2193,7 @@
         <v>64</v>
       </c>
       <c r="N6" s="156">
-        <v>0.78472222222222221</v>
+        <v>0.80972222222222223</v>
       </c>
       <c r="P6" s="156">
         <v>0.87152777777777779</v>
@@ -2190,7 +2210,9 @@
         <v>0</v>
       </c>
       <c r="E7" s="142"/>
-      <c r="F7" s="129"/>
+      <c r="F7" s="129">
+        <v>1</v>
+      </c>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2213,7 +2235,7 @@
         <v>90</v>
       </c>
       <c r="N7" s="156">
-        <v>0.78472222222222221</v>
+        <v>0.80972222222222223</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>130</v>
@@ -2226,8 +2248,12 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="34"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="34">
+        <v>50</v>
+      </c>
+      <c r="F8" s="39">
+        <v>10</v>
+      </c>
       <c r="G8" s="9" t="s">
         <v>72</v>
       </c>
@@ -2250,7 +2276,7 @@
         <v>69</v>
       </c>
       <c r="N8" s="156">
-        <v>0.78472222222222221</v>
+        <v>0.80972222222222223</v>
       </c>
       <c r="P8" s="156"/>
       <c r="R8" s="25" t="s">
@@ -2263,10 +2289,12 @@
       </c>
       <c r="B9" s="8">
         <f>7000-C2</f>
-        <v>5495</v>
+        <v>5987</v>
       </c>
       <c r="E9" s="34"/>
-      <c r="F9" s="128"/>
+      <c r="F9" s="128">
+        <v>25</v>
+      </c>
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
@@ -2289,16 +2317,18 @@
         <v>64</v>
       </c>
       <c r="N9" s="156">
-        <v>0.78472222222222221</v>
+        <v>0.80972222222222223</v>
       </c>
       <c r="P9" s="80"/>
       <c r="R9" s="25" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E10" s="34"/>
-      <c r="F10" s="39"/>
+      <c r="F10" s="39">
+        <v>12</v>
+      </c>
       <c r="G10" s="9" t="s">
         <v>81</v>
       </c>
@@ -2321,9 +2351,11 @@
         <v>66</v>
       </c>
       <c r="N10" s="156">
-        <v>0.78472222222222221</v>
-      </c>
-      <c r="P10" s="80"/>
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="P10" s="156">
+        <v>0.80972222222222223</v>
+      </c>
       <c r="R10" s="25" t="s">
         <v>141</v>
       </c>
@@ -2336,7 +2368,9 @@
         <f>B9-B13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="142"/>
+      <c r="E11" s="142">
+        <v>100</v>
+      </c>
       <c r="F11" s="39"/>
       <c r="G11" s="9" t="s">
         <v>128</v>
@@ -2348,19 +2382,19 @@
         <v>116</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="K11" s="145" t="s">
         <v>110</v>
       </c>
       <c r="L11" s="152" t="s">
-        <v>33</v>
+        <v>144</v>
       </c>
       <c r="M11" s="153" t="s">
         <v>66</v>
       </c>
       <c r="N11" s="156">
-        <v>0.78472222222222221</v>
+        <v>0.80972222222222223</v>
       </c>
       <c r="O11" s="1" t="s">
         <v>126</v>
@@ -2373,13 +2407,13 @@
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="173" t="s">
+      <c r="E12" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="174"/>
+      <c r="F12" s="173"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>20</v>
+        <v>512</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
@@ -2392,15 +2426,15 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>5495</v>
+        <v>5987</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="121"/>
-      <c r="J13" s="166"/>
+      <c r="J13" s="165"/>
       <c r="L13"/>
       <c r="M13"/>
-      <c r="N13" s="167"/>
-      <c r="O13" s="168"/>
+      <c r="N13" s="166"/>
+      <c r="O13" s="167"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
@@ -2408,11 +2442,11 @@
       <c r="E14" s="24"/>
       <c r="F14" s="20"/>
       <c r="I14" s="121"/>
-      <c r="J14" s="166"/>
+      <c r="J14" s="165"/>
       <c r="L14"/>
       <c r="M14"/>
-      <c r="N14" s="167"/>
-      <c r="O14" s="168"/>
+      <c r="N14" s="166"/>
+      <c r="O14" s="167"/>
     </row>
     <row r="15" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2426,12 +2460,12 @@
       <c r="E15" s="24"/>
       <c r="F15" s="20"/>
       <c r="I15" s="121"/>
-      <c r="J15" s="166"/>
+      <c r="J15" s="165"/>
       <c r="K15" s="121"/>
       <c r="L15"/>
       <c r="M15"/>
-      <c r="N15" s="167"/>
-      <c r="O15" s="168"/>
+      <c r="N15" s="166"/>
+      <c r="O15" s="167"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C16" s="25"/>
@@ -2450,8 +2484,8 @@
       <c r="I17" s="121"/>
       <c r="L17"/>
       <c r="M17"/>
-      <c r="N17" s="167"/>
-      <c r="O17" s="168"/>
+      <c r="N17" s="166"/>
+      <c r="O17" s="167"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2464,14 +2498,14 @@
       <c r="D18" s="25"/>
       <c r="E18" s="24"/>
       <c r="F18" s="20"/>
-      <c r="J18" s="166"/>
+      <c r="J18" s="165"/>
       <c r="L18"/>
       <c r="M18"/>
-      <c r="N18" s="167"/>
-      <c r="O18" s="168"/>
+      <c r="N18" s="166"/>
+      <c r="O18" s="167"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="J19" s="166"/>
+      <c r="J19" s="165"/>
       <c r="L19"/>
       <c r="M19"/>
     </row>
@@ -2493,7 +2527,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O28"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
@@ -2519,18 +2553,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="191" t="s">
+      <c r="E1" s="174" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="192"/>
+      <c r="F1" s="175"/>
       <c r="G1" s="43" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="191" t="s">
+      <c r="H1" s="174" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="193"/>
-      <c r="J1" s="192"/>
+      <c r="I1" s="176"/>
+      <c r="J1" s="175"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2548,7 +2582,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="178">
+      <c r="B2" s="177">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2575,26 +2609,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="194">
+      <c r="K2" s="180">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="196">
+      <c r="L2" s="182">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="181">
+      <c r="M2" s="184">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J28)</f>
-        <v>5455</v>
+        <f>SUM(E2:J29)</f>
+        <v>5947</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="180"/>
+      <c r="B3" s="178"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2609,9 +2643,9 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="57"/>
-      <c r="K3" s="195"/>
-      <c r="L3" s="197"/>
-      <c r="M3" s="182"/>
+      <c r="K3" s="181"/>
+      <c r="L3" s="183"/>
+      <c r="M3" s="185"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
@@ -2630,9 +2664,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="195"/>
-      <c r="L4" s="197"/>
-      <c r="M4" s="182"/>
+      <c r="K4" s="181"/>
+      <c r="L4" s="183"/>
+      <c r="M4" s="185"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2714,7 +2748,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="183">
+      <c r="B7" s="186">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2731,22 +2765,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="185">
+      <c r="K7" s="188">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="187">
+      <c r="L7" s="190">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="189">
+      <c r="M7" s="192">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="184"/>
+      <c r="B8" s="187"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2767,9 +2801,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="186"/>
-      <c r="L8" s="188"/>
-      <c r="M8" s="190"/>
+      <c r="K8" s="189"/>
+      <c r="L8" s="191"/>
+      <c r="M8" s="193"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2849,7 +2883,7 @@
       <c r="A11" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="183">
+      <c r="B11" s="186">
         <v>8</v>
       </c>
       <c r="C11" s="70"/>
@@ -2876,7 +2910,7 @@
       <c r="M11" s="72"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="184"/>
+      <c r="B12" s="187"/>
       <c r="C12" s="92">
         <v>483</v>
       </c>
@@ -2933,7 +2967,7 @@
       <c r="M13" s="84"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="183">
+      <c r="B14" s="186">
         <v>10</v>
       </c>
       <c r="C14" s="97"/>
@@ -2956,7 +2990,7 @@
       <c r="A15" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="184"/>
+      <c r="B15" s="187"/>
       <c r="C15" s="98"/>
       <c r="D15" s="84">
         <v>175</v>
@@ -2980,7 +3014,7 @@
       <c r="M15" s="93"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="178">
+      <c r="B16" s="177">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3011,7 +3045,7 @@
       <c r="A17" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="180"/>
+      <c r="B17" s="178"/>
       <c r="C17" s="84"/>
       <c r="D17" s="84"/>
       <c r="E17" s="84"/>
@@ -3029,7 +3063,7 @@
       <c r="M17" s="84"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="178">
+      <c r="B18" s="177">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3118,7 +3152,7 @@
       <c r="A21" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="176">
+      <c r="B21" s="195">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3146,7 +3180,7 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="177"/>
+      <c r="B22" s="196"/>
       <c r="C22" s="133"/>
       <c r="D22" s="134">
         <v>235</v>
@@ -3198,7 +3232,7 @@
       <c r="M23" s="72"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="171">
+      <c r="B24" s="170">
         <v>16</v>
       </c>
       <c r="C24" s="143"/>
@@ -3227,7 +3261,7 @@
       <c r="A25" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="172"/>
+      <c r="B25" s="171"/>
       <c r="C25" s="144"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -3255,7 +3289,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="171">
+      <c r="B26" s="170">
         <v>17</v>
       </c>
       <c r="C26" s="164"/>
@@ -3286,7 +3320,7 @@
       <c r="A27" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="175"/>
+      <c r="B27" s="194"/>
       <c r="C27" s="98"/>
       <c r="D27" s="134">
         <v>100</v>
@@ -3317,32 +3351,61 @@
       <c r="A28" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="165">
+      <c r="B28" s="170">
         <v>18</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="59"/>
-      <c r="E28" s="59"/>
-      <c r="F28" s="59"/>
-      <c r="G28" s="59"/>
-      <c r="H28" s="59">
+      <c r="C28" s="143"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71">
         <v>10</v>
       </c>
-      <c r="I28" s="59">
+      <c r="I28" s="71">
         <v>10</v>
       </c>
-      <c r="J28" s="59"/>
-      <c r="K28" s="59"/>
-      <c r="L28" s="59"/>
-      <c r="M28" s="60"/>
+      <c r="J28" s="71">
+        <v>12</v>
+      </c>
+      <c r="K28" s="71"/>
+      <c r="L28" s="71"/>
+      <c r="M28" s="72"/>
+    </row>
+    <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="197"/>
+      <c r="C29" s="18"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="198">
+        <v>222</v>
+      </c>
+      <c r="F29" s="198">
+        <v>50</v>
+      </c>
+      <c r="G29" s="198">
+        <v>100</v>
+      </c>
+      <c r="H29" s="198">
+        <v>63</v>
+      </c>
+      <c r="I29" s="198">
+        <v>25</v>
+      </c>
+      <c r="J29" s="198">
+        <v>20</v>
+      </c>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
+  <mergeCells count="18">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B16:B17"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B11:B12"/>
@@ -3350,11 +3413,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6561,10 +6624,10 @@
       <c r="CG23" s="51"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="173" t="s">
+      <c r="AG24" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="174"/>
+      <c r="AH24" s="173"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -6584,10 +6647,10 @@
       <c r="AV24" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="173" t="s">
+      <c r="AZ24" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="174"/>
+      <c r="BA24" s="173"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -6607,10 +6670,10 @@
       <c r="BO24" s="53" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="173" t="s">
+      <c r="BR24" s="172" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="174"/>
+      <c r="BS24" s="173"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>

</xml_diff>

<commit_message>
Rw-NewDelhi Usage - Enabled
Rw-NewDelhi Usage_18122023
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05727EAB-9323-4D06-8219-F1B6DFB057F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D927064E-D2C5-4DB3-9C63-4CA34F7736D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="145">
   <si>
     <t>UnSettled</t>
   </si>
@@ -462,9 +462,6 @@
   </si>
   <si>
     <t>19/12/2023</t>
-  </si>
-  <si>
-    <t>Rw- Mumbai</t>
   </si>
   <si>
     <t>TBS News</t>
@@ -1226,7 +1223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1687,6 +1684,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1696,10 +1696,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1983,7 +1979,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="J13" sqref="J13:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2105,7 +2101,7 @@
         <v>133</v>
       </c>
       <c r="K4" s="145" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="L4" s="147" t="s">
         <v>94</v>
@@ -2321,7 +2317,7 @@
       </c>
       <c r="P9" s="80"/>
       <c r="R9" s="25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2382,13 +2378,13 @@
         <v>116</v>
       </c>
       <c r="J11" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="K11" s="145" t="s">
         <v>110</v>
       </c>
       <c r="L11" s="152" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="M11" s="153" t="s">
         <v>66</v>
@@ -3152,7 +3148,7 @@
       <c r="A21" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="195">
+      <c r="B21" s="196">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3180,7 +3176,7 @@
       <c r="M21" s="57"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="196"/>
+      <c r="B22" s="197"/>
       <c r="C22" s="133"/>
       <c r="D22" s="134">
         <v>235</v>
@@ -3320,7 +3316,7 @@
       <c r="A27" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="194"/>
+      <c r="B27" s="195"/>
       <c r="C27" s="98"/>
       <c r="D27" s="134">
         <v>100</v>
@@ -3373,25 +3369,25 @@
       <c r="M28" s="72"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="197"/>
+      <c r="B29" s="194"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
-      <c r="E29" s="198">
+      <c r="E29" s="18">
         <v>222</v>
       </c>
-      <c r="F29" s="198">
+      <c r="F29" s="18">
         <v>50</v>
       </c>
-      <c r="G29" s="198">
+      <c r="G29" s="18">
         <v>100</v>
       </c>
-      <c r="H29" s="198">
+      <c r="H29" s="18">
         <v>63</v>
       </c>
-      <c r="I29" s="198">
+      <c r="I29" s="18">
         <v>25</v>
       </c>
-      <c r="J29" s="198">
+      <c r="J29" s="18">
         <v>20</v>
       </c>
       <c r="K29" s="18"/>

</xml_diff>

<commit_message>
Rw Usage Updates_19122023 11:38 AM
Rw Usage Updates_19122023 11:38 AM

Boat Enabled
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B6C0E2-6188-4730-97C8-AC055AE47D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{851E4F33-D489-4CF1-B151-AEC2B9ED215C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dashboard" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="147">
   <si>
     <t>UnSettled</t>
   </si>
@@ -1229,7 +1229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1633,26 +1633,35 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1684,27 +1693,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1987,8 +2009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2068,7 +2090,7 @@
       </c>
       <c r="T2" s="98">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
+        <v>45279</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2094,9 +2116,7 @@
       <c r="E4" s="161">
         <v>10</v>
       </c>
-      <c r="F4" s="37">
-        <v>42</v>
-      </c>
+      <c r="F4" s="37"/>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -2119,13 +2139,13 @@
         <v>30</v>
       </c>
       <c r="N4" s="154">
-        <v>0.80972222222222223</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="P4" s="154">
         <v>0.87152777777777779</v>
       </c>
       <c r="R4" s="25" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2133,11 +2153,9 @@
         <v>-2</v>
       </c>
       <c r="E5" s="133">
-        <v>10</v>
-      </c>
-      <c r="F5" s="126">
         <v>20</v>
       </c>
+      <c r="F5" s="126"/>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2160,22 +2178,20 @@
         <v>86</v>
       </c>
       <c r="N5" s="154">
-        <v>0.80972222222222223</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="P5" s="154">
         <v>0.87152777777777779</v>
       </c>
       <c r="R5" s="25" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="133">
-        <v>222</v>
-      </c>
-      <c r="F6" s="127">
-        <v>10</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="F6" s="127"/>
       <c r="G6" s="28" t="s">
         <v>135</v>
       </c>
@@ -2198,13 +2214,13 @@
         <v>64</v>
       </c>
       <c r="N6" s="154">
-        <v>0.46527777777777773</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="P6" s="154">
         <v>0.87152777777777779</v>
       </c>
       <c r="R6" s="25" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2214,10 +2230,10 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="140"/>
-      <c r="F7" s="127">
-        <v>1</v>
-      </c>
+      <c r="E7" s="140">
+        <v>5</v>
+      </c>
+      <c r="F7" s="127"/>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2240,7 +2256,7 @@
         <v>90</v>
       </c>
       <c r="N7" s="154">
-        <v>0.80972222222222223</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>130</v>
@@ -2249,16 +2265,12 @@
         <v>0.78472222222222221</v>
       </c>
       <c r="R7" s="25" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="33">
-        <v>50</v>
-      </c>
-      <c r="F8" s="37">
-        <v>10</v>
-      </c>
+      <c r="E8" s="33"/>
+      <c r="F8" s="37"/>
       <c r="G8" s="9" t="s">
         <v>72</v>
       </c>
@@ -2280,12 +2292,10 @@
       <c r="M8" s="148" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="154">
-        <v>0.80972222222222223</v>
-      </c>
+      <c r="N8" s="154"/>
       <c r="P8" s="154"/>
       <c r="R8" s="25" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2297,9 +2307,7 @@
         <v>5987</v>
       </c>
       <c r="E9" s="33"/>
-      <c r="F9" s="126">
-        <v>25</v>
-      </c>
+      <c r="F9" s="126"/>
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
@@ -2321,19 +2329,17 @@
       <c r="M9" s="148" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="154">
-        <v>0.80972222222222223</v>
-      </c>
+      <c r="N9" s="154"/>
       <c r="P9" s="78"/>
       <c r="R9" s="25" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="33"/>
-      <c r="F10" s="37">
-        <v>12</v>
-      </c>
+      <c r="E10" s="33">
+        <v>70</v>
+      </c>
+      <c r="F10" s="37"/>
       <c r="G10" s="9" t="s">
         <v>81</v>
       </c>
@@ -2356,13 +2362,16 @@
         <v>66</v>
       </c>
       <c r="N10" s="154">
-        <v>0.80972222222222223</v>
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="O10" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="P10" s="154">
-        <v>0.80972222222222223</v>
+        <v>0.4826388888888889</v>
       </c>
       <c r="R10" s="25" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2371,11 +2380,9 @@
       </c>
       <c r="B11" s="8">
         <f>B9-B13</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="140">
-        <v>100</v>
-      </c>
+        <v>-110</v>
+      </c>
+      <c r="E11" s="140"/>
       <c r="F11" s="37"/>
       <c r="G11" s="9" t="s">
         <v>128</v>
@@ -2398,17 +2405,12 @@
       <c r="M11" s="151" t="s">
         <v>66</v>
       </c>
-      <c r="N11" s="154">
-        <v>0.80972222222222223</v>
-      </c>
-      <c r="O11" s="1" t="s">
-        <v>126</v>
-      </c>
+      <c r="N11" s="154"/>
       <c r="P11" s="154">
         <v>0.78472222222222221</v>
       </c>
       <c r="R11" s="25" t="s">
-        <v>138</v>
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2418,7 +2420,7 @@
       <c r="F12" s="172"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>512</v>
+        <v>110</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
@@ -2431,7 +2433,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>5987</v>
+        <v>6097</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="119"/>
@@ -2533,10 +2535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O29"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="R9" sqref="R9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2559,18 +2561,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="192" t="s">
+      <c r="E1" s="175" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="193"/>
+      <c r="F1" s="176"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="192" t="s">
+      <c r="H1" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="194"/>
-      <c r="J1" s="193"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="176"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2588,7 +2590,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="179">
+      <c r="B2" s="178">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2615,26 +2617,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="195">
+      <c r="K2" s="181">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="197">
+      <c r="L2" s="183">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="182">
+      <c r="M2" s="185">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J29)</f>
-        <v>5947</v>
+        <f>SUM(E2:J30)</f>
+        <v>6057</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="181"/>
+      <c r="B3" s="179"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2649,9 +2651,9 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="198"/>
-      <c r="M3" s="183"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="186"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
@@ -2670,9 +2672,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="196"/>
-      <c r="L4" s="198"/>
-      <c r="M4" s="183"/>
+      <c r="K4" s="182"/>
+      <c r="L4" s="184"/>
+      <c r="M4" s="186"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2754,7 +2756,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="184">
+      <c r="B7" s="187">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2771,22 +2773,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="186">
+      <c r="K7" s="189">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="188">
+      <c r="L7" s="191">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="190">
+      <c r="M7" s="193">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="185"/>
+      <c r="B8" s="188"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2807,9 +2809,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="187"/>
-      <c r="L8" s="189"/>
-      <c r="M8" s="191"/>
+      <c r="K8" s="190"/>
+      <c r="L8" s="192"/>
+      <c r="M8" s="194"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2889,7 +2891,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="184">
+      <c r="B11" s="187">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -2916,7 +2918,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="185"/>
+      <c r="B12" s="188"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -2973,7 +2975,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="184">
+      <c r="B14" s="187">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -2996,7 +2998,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="185"/>
+      <c r="B15" s="188"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3020,7 +3022,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="179">
+      <c r="B16" s="178">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3051,7 +3053,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="181"/>
+      <c r="B17" s="179"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3069,7 +3071,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="179">
+      <c r="B18" s="178">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3158,7 +3160,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="177">
+      <c r="B21" s="197">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3186,7 +3188,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="178"/>
+      <c r="B22" s="198"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -3326,7 +3328,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="176"/>
+      <c r="B27" s="196"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -3379,7 +3381,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="175"/>
+      <c r="B29" s="195"/>
       <c r="C29" s="18"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -3404,13 +3406,33 @@
       <c r="L29" s="18"/>
       <c r="M29" s="18"/>
     </row>
+    <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="130">
+        <v>19</v>
+      </c>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="208">
+        <v>70</v>
+      </c>
+      <c r="H30" s="208">
+        <v>40</v>
+      </c>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="B14:B15"/>
@@ -3419,11 +3441,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3431,10 +3453,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EF39B9-450C-4C51-9807-7AFD5CC29C14}">
-  <dimension ref="A1:CG24"/>
+  <dimension ref="A1:CG36"/>
   <sheetViews>
-    <sheetView topLeftCell="BN6" workbookViewId="0">
-      <selection activeCell="BP15" sqref="BP15"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="U31" sqref="U31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4984,7 +5006,7 @@
       </c>
       <c r="AC14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
+        <v>45279</v>
       </c>
       <c r="AG14" s="99" t="s">
         <v>44</v>
@@ -5029,7 +5051,7 @@
       <c r="AU14" s="43"/>
       <c r="AV14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
+        <v>45279</v>
       </c>
       <c r="AZ14" s="99" t="s">
         <v>44</v>
@@ -5074,7 +5096,7 @@
       <c r="BN14" s="43"/>
       <c r="BO14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
+        <v>45279</v>
       </c>
       <c r="BR14" s="159" t="s">
         <v>44</v>
@@ -5119,7 +5141,7 @@
       <c r="CF14" s="43"/>
       <c r="CG14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45278</v>
+        <v>45279</v>
       </c>
     </row>
     <row r="15" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6700,11 +6722,407 @@
         <v>134</v>
       </c>
     </row>
+    <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="173" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="174"/>
+      <c r="D26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="I26" s="125" t="s">
+        <v>38</v>
+      </c>
+      <c r="J26" s="125" t="s">
+        <v>92</v>
+      </c>
+      <c r="K26" s="153" t="s">
+        <v>68</v>
+      </c>
+      <c r="L26" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="M26" s="157" t="s">
+        <v>83</v>
+      </c>
+      <c r="N26" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="O26" s="26" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="136"/>
+      <c r="C27" s="199"/>
+      <c r="D27" s="200"/>
+      <c r="E27" s="201"/>
+      <c r="F27" s="202"/>
+      <c r="G27" s="199"/>
+      <c r="H27" s="200"/>
+      <c r="I27" s="203"/>
+      <c r="J27" s="203"/>
+      <c r="K27" s="204"/>
+      <c r="L27" s="203"/>
+      <c r="M27" s="203"/>
+      <c r="N27" s="203"/>
+      <c r="O27" s="101"/>
+    </row>
+    <row r="28" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="161">
+        <v>10</v>
+      </c>
+      <c r="C28" s="37">
+        <v>42</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="F28" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="G28" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="H28" s="143" t="s">
+        <v>118</v>
+      </c>
+      <c r="I28" s="145" t="s">
+        <v>146</v>
+      </c>
+      <c r="J28" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="K28" s="205">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="L28" s="203"/>
+      <c r="M28" s="205">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="N28" s="203"/>
+      <c r="O28" s="101" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="133">
+        <v>10</v>
+      </c>
+      <c r="C29" s="126">
+        <v>20</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="E29" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="F29" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="I29" s="147" t="s">
+        <v>137</v>
+      </c>
+      <c r="J29" s="148" t="s">
+        <v>86</v>
+      </c>
+      <c r="K29" s="205">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="L29" s="203"/>
+      <c r="M29" s="205">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="N29" s="203"/>
+      <c r="O29" s="101" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="30" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="133">
+        <v>222</v>
+      </c>
+      <c r="C30" s="127">
+        <v>10</v>
+      </c>
+      <c r="D30" s="206" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="120" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="G30" s="37" t="s">
+        <v>102</v>
+      </c>
+      <c r="H30" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="I30" s="145" t="s">
+        <v>96</v>
+      </c>
+      <c r="J30" s="148" t="s">
+        <v>64</v>
+      </c>
+      <c r="K30" s="205">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="L30" s="203"/>
+      <c r="M30" s="205">
+        <v>0.87152777777777779</v>
+      </c>
+      <c r="N30" s="203"/>
+      <c r="O30" s="101" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="140"/>
+      <c r="C31" s="127">
+        <v>1</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E31" s="124" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="G31" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H31" s="143" t="s">
+        <v>91</v>
+      </c>
+      <c r="I31" s="149" t="s">
+        <v>85</v>
+      </c>
+      <c r="J31" s="148" t="s">
+        <v>90</v>
+      </c>
+      <c r="K31" s="205">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="L31" s="203" t="s">
+        <v>130</v>
+      </c>
+      <c r="M31" s="205">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="N31" s="203"/>
+      <c r="O31" s="101" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="32" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="33">
+        <v>50</v>
+      </c>
+      <c r="C32" s="37">
+        <v>10</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E32" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="G32" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="H32" s="143" t="s">
+        <v>121</v>
+      </c>
+      <c r="I32" s="149" t="s">
+        <v>123</v>
+      </c>
+      <c r="J32" s="148" t="s">
+        <v>69</v>
+      </c>
+      <c r="K32" s="205">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="L32" s="203"/>
+      <c r="M32" s="205"/>
+      <c r="N32" s="203"/>
+      <c r="O32" s="101" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="33"/>
+      <c r="C33" s="126">
+        <v>25</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E33" s="156" t="s">
+        <v>17</v>
+      </c>
+      <c r="F33" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="G33" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="H33" s="143" t="s">
+        <v>129</v>
+      </c>
+      <c r="I33" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="J33" s="148" t="s">
+        <v>64</v>
+      </c>
+      <c r="K33" s="205">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="L33" s="203"/>
+      <c r="M33" s="207"/>
+      <c r="N33" s="203"/>
+      <c r="O33" s="101" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="33"/>
+      <c r="C34" s="37">
+        <v>12</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E34" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="G34" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="H34" s="144" t="s">
+        <v>122</v>
+      </c>
+      <c r="I34" s="149" t="s">
+        <v>124</v>
+      </c>
+      <c r="J34" s="148" t="s">
+        <v>66</v>
+      </c>
+      <c r="K34" s="205">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="L34" s="203"/>
+      <c r="M34" s="205">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="N34" s="203"/>
+      <c r="O34" s="101" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="140">
+        <v>100</v>
+      </c>
+      <c r="C35" s="37"/>
+      <c r="D35" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="E35" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="F35" s="118" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="H35" s="143" t="s">
+        <v>110</v>
+      </c>
+      <c r="I35" s="150" t="s">
+        <v>143</v>
+      </c>
+      <c r="J35" s="151" t="s">
+        <v>66</v>
+      </c>
+      <c r="K35" s="205">
+        <v>0.80972222222222223</v>
+      </c>
+      <c r="L35" s="203" t="s">
+        <v>126</v>
+      </c>
+      <c r="M35" s="205">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="N35" s="203"/>
+      <c r="O35" s="101" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="171" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" s="172"/>
+      <c r="D36" s="9">
+        <f>SUM(B28:C35)</f>
+        <v>512</v>
+      </c>
+      <c r="E36" s="114"/>
+      <c r="F36" s="137"/>
+      <c r="G36" s="79" t="s">
+        <v>138</v>
+      </c>
+      <c r="H36" s="50"/>
+      <c r="I36" s="138"/>
+      <c r="J36" s="50"/>
+      <c r="K36" s="158"/>
+      <c r="L36" s="115"/>
+      <c r="M36" s="65"/>
+      <c r="N36" s="65"/>
+      <c r="O36" s="102"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
     <mergeCell ref="BR24:BS24"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Update Usage Report_19122023
Rw Update Usage Report
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08F4380-410B-4B3D-A1F2-38C281975590}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D558B9-7FE9-4628-82A1-FB977AE12F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="148">
   <si>
     <t>UnSettled</t>
   </si>
@@ -1232,7 +1232,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="198">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1636,26 +1636,35 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1687,25 +1696,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1991,7 +1988,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O13" sqref="O13:O15"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,7 +2024,7 @@
       </c>
       <c r="C2" s="169">
         <f>B3+B4</f>
-        <v>903</v>
+        <v>831</v>
       </c>
       <c r="E2" s="173" t="s">
         <v>145</v>
@@ -2089,7 +2086,7 @@
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="168"/>
       <c r="B4" s="34">
-        <v>403</v>
+        <v>331</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>35</v>
@@ -2097,7 +2094,9 @@
       <c r="E4" s="161">
         <v>10</v>
       </c>
-      <c r="F4" s="37"/>
+      <c r="F4" s="37">
+        <v>10</v>
+      </c>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -2120,10 +2119,10 @@
         <v>30</v>
       </c>
       <c r="N4" s="154">
-        <v>0.4826388888888889</v>
+        <v>0.8208333333333333</v>
       </c>
       <c r="P4" s="154">
-        <v>0.87152777777777779</v>
+        <v>0.8208333333333333</v>
       </c>
       <c r="R4" s="25" t="s">
         <v>144</v>
@@ -2136,7 +2135,9 @@
       <c r="E5" s="133">
         <v>20</v>
       </c>
-      <c r="F5" s="126"/>
+      <c r="F5" s="126">
+        <v>20</v>
+      </c>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2159,10 +2160,10 @@
         <v>86</v>
       </c>
       <c r="N5" s="154">
-        <v>0.4826388888888889</v>
+        <v>0.8208333333333333</v>
       </c>
       <c r="P5" s="154">
-        <v>0.87152777777777779</v>
+        <v>0.8208333333333333</v>
       </c>
       <c r="R5" s="25" t="s">
         <v>144</v>
@@ -2172,7 +2173,9 @@
       <c r="E6" s="133">
         <v>5</v>
       </c>
-      <c r="F6" s="127"/>
+      <c r="F6" s="127">
+        <v>20</v>
+      </c>
       <c r="G6" s="28" t="s">
         <v>147</v>
       </c>
@@ -2195,10 +2198,10 @@
         <v>64</v>
       </c>
       <c r="N6" s="154">
-        <v>0.4826388888888889</v>
+        <v>0.8208333333333333</v>
       </c>
       <c r="P6" s="154">
-        <v>0.87152777777777779</v>
+        <v>0.8208333333333333</v>
       </c>
       <c r="R6" s="25" t="s">
         <v>144</v>
@@ -2251,7 +2254,9 @@
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="33"/>
-      <c r="F8" s="37"/>
+      <c r="F8" s="37">
+        <v>10</v>
+      </c>
       <c r="G8" s="9" t="s">
         <v>72</v>
       </c>
@@ -2273,8 +2278,12 @@
       <c r="M8" s="148" t="s">
         <v>69</v>
       </c>
-      <c r="N8" s="154"/>
-      <c r="P8" s="154"/>
+      <c r="N8" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="P8" s="154">
+        <v>0.8208333333333333</v>
+      </c>
       <c r="R8" s="25" t="s">
         <v>144</v>
       </c>
@@ -2285,10 +2294,12 @@
       </c>
       <c r="B9" s="8">
         <f>7000-C2</f>
-        <v>6097</v>
+        <v>6169</v>
       </c>
       <c r="E9" s="33"/>
-      <c r="F9" s="126"/>
+      <c r="F9" s="126">
+        <v>10</v>
+      </c>
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
@@ -2310,8 +2321,12 @@
       <c r="M9" s="148" t="s">
         <v>64</v>
       </c>
-      <c r="N9" s="154"/>
-      <c r="P9" s="78"/>
+      <c r="N9" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="P9" s="154">
+        <v>0.8208333333333333</v>
+      </c>
       <c r="R9" s="25" t="s">
         <v>144</v>
       </c>
@@ -2364,7 +2379,9 @@
         <v>0</v>
       </c>
       <c r="E11" s="140"/>
-      <c r="F11" s="37"/>
+      <c r="F11" s="37">
+        <v>2</v>
+      </c>
       <c r="G11" s="9" t="s">
         <v>128</v>
       </c>
@@ -2386,7 +2403,9 @@
       <c r="M11" s="151" t="s">
         <v>66</v>
       </c>
-      <c r="N11" s="154"/>
+      <c r="N11" s="154">
+        <v>0.8208333333333333</v>
+      </c>
       <c r="P11" s="154">
         <v>0.78472222222222221</v>
       </c>
@@ -2401,7 +2420,7 @@
       <c r="F12" s="172"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>110</v>
+        <v>182</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
@@ -2414,7 +2433,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>6097</v>
+        <v>6169</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="119"/>
@@ -2516,10 +2535,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O30"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2542,18 +2561,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="192" t="s">
+      <c r="E1" s="175" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="193"/>
+      <c r="F1" s="176"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="192" t="s">
+      <c r="H1" s="175" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="194"/>
-      <c r="J1" s="193"/>
+      <c r="I1" s="177"/>
+      <c r="J1" s="176"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2571,7 +2590,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="179">
+      <c r="B2" s="178">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2598,26 +2617,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="195">
+      <c r="K2" s="181">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="197">
+      <c r="L2" s="183">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="182">
+      <c r="M2" s="185">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J30)</f>
-        <v>6057</v>
+        <f>SUM(E2:J31)</f>
+        <v>6129</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="181"/>
+      <c r="B3" s="179"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2632,9 +2651,9 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="196"/>
-      <c r="L3" s="198"/>
-      <c r="M3" s="183"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="184"/>
+      <c r="M3" s="186"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
@@ -2653,9 +2672,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="196"/>
-      <c r="L4" s="198"/>
-      <c r="M4" s="183"/>
+      <c r="K4" s="182"/>
+      <c r="L4" s="184"/>
+      <c r="M4" s="186"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2737,7 +2756,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="184">
+      <c r="B7" s="187">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2754,22 +2773,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="186">
+      <c r="K7" s="189">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="188">
+      <c r="L7" s="191">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="190">
+      <c r="M7" s="193">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="185"/>
+      <c r="B8" s="188"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2790,9 +2809,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="187"/>
-      <c r="L8" s="189"/>
-      <c r="M8" s="191"/>
+      <c r="K8" s="190"/>
+      <c r="L8" s="192"/>
+      <c r="M8" s="194"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2872,7 +2891,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="184">
+      <c r="B11" s="187">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -2899,7 +2918,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="185"/>
+      <c r="B12" s="188"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -2956,7 +2975,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="184">
+      <c r="B14" s="187">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -2979,7 +2998,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="185"/>
+      <c r="B15" s="188"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3003,7 +3022,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="179">
+      <c r="B16" s="178">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3034,7 +3053,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="181"/>
+      <c r="B17" s="179"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3052,7 +3071,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="179">
+      <c r="B18" s="178">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3141,7 +3160,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="177">
+      <c r="B21" s="196">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3169,7 +3188,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="178"/>
+      <c r="B22" s="197"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -3309,7 +3328,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="176"/>
+      <c r="B27" s="195"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -3362,8 +3381,8 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="175"/>
-      <c r="C29" s="18"/>
+      <c r="B29" s="170"/>
+      <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
         <v>222</v>
@@ -3388,10 +3407,10 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="130">
+      <c r="B30" s="169">
         <v>19</v>
       </c>
-      <c r="C30" s="18"/>
+      <c r="C30" s="142"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
       <c r="F30" s="18"/>
@@ -3407,13 +3426,41 @@
       <c r="L30" s="18"/>
       <c r="M30" s="18"/>
     </row>
+    <row r="31" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31" s="170"/>
+      <c r="C31" s="142"/>
+      <c r="D31" s="18"/>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18">
+        <v>20</v>
+      </c>
+      <c r="G31" s="18">
+        <v>20</v>
+      </c>
+      <c r="H31" s="18">
+        <v>20</v>
+      </c>
+      <c r="I31" s="18">
+        <v>10</v>
+      </c>
+      <c r="J31" s="18">
+        <v>2</v>
+      </c>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="18"/>
+    </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
+  <mergeCells count="19">
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B18:B19"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="M2:M4"/>
     <mergeCell ref="B14:B15"/>
@@ -3422,11 +3469,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Updates - Usage Report_11:52AM
Rw Updates - Usage Report - 20/12/2023
Boat Enabled ,

[12F Reserved] - [4F Mapped]
Boat Matrix - [-9]yd + [-4]td + (-3)ed
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7D558B9-7FE9-4628-82A1-FB977AE12F07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76307650-E213-45A5-A5E8-CE4565E1F070}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="149">
   <si>
     <t>UnSettled</t>
   </si>
@@ -480,13 +480,16 @@
   </si>
   <si>
     <t>Food /BeeHub</t>
+  </si>
+  <si>
+    <t>21/12/2023</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,6 +594,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1232,7 +1243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="198">
+  <cellXfs count="200">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1636,36 +1647,24 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1696,13 +1695,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1988,7 +2003,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,7 +2039,7 @@
       </c>
       <c r="C2" s="169">
         <f>B3+B4</f>
-        <v>831</v>
+        <v>711</v>
       </c>
       <c r="E2" s="173" t="s">
         <v>145</v>
@@ -2068,7 +2083,7 @@
       </c>
       <c r="T2" s="98">
         <f ca="1">TODAY()</f>
-        <v>45279</v>
+        <v>45280</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2086,7 +2101,7 @@
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="168"/>
       <c r="B4" s="34">
-        <v>331</v>
+        <v>211</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>35</v>
@@ -2094,9 +2109,7 @@
       <c r="E4" s="161">
         <v>10</v>
       </c>
-      <c r="F4" s="37">
-        <v>10</v>
-      </c>
+      <c r="F4" s="37"/>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -2119,7 +2132,7 @@
         <v>30</v>
       </c>
       <c r="N4" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="P4" s="154">
         <v>0.8208333333333333</v>
@@ -2135,9 +2148,7 @@
       <c r="E5" s="133">
         <v>20</v>
       </c>
-      <c r="F5" s="126">
-        <v>20</v>
-      </c>
+      <c r="F5" s="126"/>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2160,7 +2171,7 @@
         <v>86</v>
       </c>
       <c r="N5" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="P5" s="154">
         <v>0.8208333333333333</v>
@@ -2171,11 +2182,9 @@
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="133">
-        <v>5</v>
-      </c>
-      <c r="F6" s="127">
-        <v>20</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F6" s="127"/>
       <c r="G6" s="28" t="s">
         <v>147</v>
       </c>
@@ -2198,7 +2207,7 @@
         <v>64</v>
       </c>
       <c r="N6" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="P6" s="154">
         <v>0.8208333333333333</v>
@@ -2215,7 +2224,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="140">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F7" s="127"/>
       <c r="G7" s="9" t="s">
@@ -2253,10 +2262,10 @@
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E8" s="33"/>
-      <c r="F8" s="37">
-        <v>10</v>
-      </c>
+      <c r="E8" s="199">
+        <v>25</v>
+      </c>
+      <c r="F8" s="37"/>
       <c r="G8" s="9" t="s">
         <v>72</v>
       </c>
@@ -2279,13 +2288,13 @@
         <v>69</v>
       </c>
       <c r="N8" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="P8" s="154">
         <v>0.8208333333333333</v>
       </c>
       <c r="R8" s="25" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2294,12 +2303,12 @@
       </c>
       <c r="B9" s="8">
         <f>7000-C2</f>
-        <v>6169</v>
-      </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="126">
-        <v>10</v>
-      </c>
+        <v>6289</v>
+      </c>
+      <c r="E9" s="199">
+        <v>25</v>
+      </c>
+      <c r="F9" s="126"/>
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
@@ -2322,18 +2331,18 @@
         <v>64</v>
       </c>
       <c r="N9" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="P9" s="154">
         <v>0.8208333333333333</v>
       </c>
       <c r="R9" s="25" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="33">
-        <v>70</v>
+      <c r="E10" s="140">
+        <v>10</v>
       </c>
       <c r="F10" s="37"/>
       <c r="G10" s="9" t="s">
@@ -2358,7 +2367,7 @@
         <v>66</v>
       </c>
       <c r="N10" s="154">
-        <v>0.4826388888888889</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>126</v>
@@ -2378,10 +2387,10 @@
         <f>B9-B13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="140"/>
-      <c r="F11" s="37">
-        <v>2</v>
-      </c>
+      <c r="E11" s="140">
+        <v>10</v>
+      </c>
+      <c r="F11" s="37"/>
       <c r="G11" s="9" t="s">
         <v>128</v>
       </c>
@@ -2404,7 +2413,7 @@
         <v>66</v>
       </c>
       <c r="N11" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.4861111111111111</v>
       </c>
       <c r="P11" s="154">
         <v>0.78472222222222221</v>
@@ -2420,7 +2429,7 @@
       <c r="F12" s="172"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>182</v>
+        <v>120</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
@@ -2433,7 +2442,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>6169</v>
+        <v>6289</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="119"/>
@@ -2535,10 +2544,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2561,18 +2570,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="175" t="s">
+      <c r="E1" s="191" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="176"/>
+      <c r="F1" s="192"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="175" t="s">
+      <c r="H1" s="191" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="177"/>
-      <c r="J1" s="176"/>
+      <c r="I1" s="193"/>
+      <c r="J1" s="192"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2617,26 +2626,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="181">
+      <c r="K2" s="194">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="183">
+      <c r="L2" s="196">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="185">
+      <c r="M2" s="181">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J31)</f>
-        <v>6129</v>
+        <f>SUM(E2:J32)</f>
+        <v>6249</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="179"/>
+      <c r="B3" s="180"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2651,13 +2660,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="182"/>
-      <c r="L3" s="184"/>
-      <c r="M3" s="186"/>
+      <c r="K3" s="195"/>
+      <c r="L3" s="197"/>
+      <c r="M3" s="182"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="180"/>
+      <c r="B4" s="179"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2672,9 +2681,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="182"/>
-      <c r="L4" s="184"/>
-      <c r="M4" s="186"/>
+      <c r="K4" s="195"/>
+      <c r="L4" s="197"/>
+      <c r="M4" s="182"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2756,7 +2765,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="187">
+      <c r="B7" s="183">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2773,22 +2782,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="189">
+      <c r="K7" s="185">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="191">
+      <c r="L7" s="187">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="193">
+      <c r="M7" s="189">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="188"/>
+      <c r="B8" s="184"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2809,9 +2818,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="190"/>
-      <c r="L8" s="192"/>
-      <c r="M8" s="194"/>
+      <c r="K8" s="186"/>
+      <c r="L8" s="188"/>
+      <c r="M8" s="190"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2891,7 +2900,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="187">
+      <c r="B11" s="183">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -2918,7 +2927,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="188"/>
+      <c r="B12" s="184"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -2975,7 +2984,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="187">
+      <c r="B14" s="183">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -2998,7 +3007,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="188"/>
+      <c r="B15" s="184"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3053,7 +3062,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="179"/>
+      <c r="B17" s="180"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3100,7 +3109,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="180"/>
+      <c r="B19" s="179"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3160,7 +3169,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="196">
+      <c r="B21" s="176">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3188,7 +3197,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="197"/>
+      <c r="B22" s="177"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -3328,7 +3337,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="195"/>
+      <c r="B27" s="175"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -3453,13 +3462,38 @@
       <c r="L31" s="18"/>
       <c r="M31" s="18"/>
     </row>
+    <row r="32" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="84" t="s">
+        <v>1</v>
+      </c>
+      <c r="B32" s="130">
+        <v>20</v>
+      </c>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="198">
+        <v>50</v>
+      </c>
+      <c r="G32" s="198"/>
+      <c r="H32" s="198">
+        <v>40</v>
+      </c>
+      <c r="I32" s="198"/>
+      <c r="J32" s="198">
+        <v>30</v>
+      </c>
+      <c r="K32" s="18"/>
+      <c r="L32" s="18"/>
+      <c r="M32" s="18"/>
+    </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="M2:M4"/>
@@ -3469,11 +3503,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B21:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3484,7 +3518,7 @@
   <dimension ref="A1:CG36"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="Q32" sqref="Q32"/>
+      <selection activeCell="R26" sqref="R26:AE36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5034,7 +5068,7 @@
       </c>
       <c r="AC14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45279</v>
+        <v>45280</v>
       </c>
       <c r="AG14" s="99" t="s">
         <v>44</v>
@@ -5079,7 +5113,7 @@
       <c r="AU14" s="43"/>
       <c r="AV14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45279</v>
+        <v>45280</v>
       </c>
       <c r="AZ14" s="99" t="s">
         <v>44</v>
@@ -5124,7 +5158,7 @@
       <c r="BN14" s="43"/>
       <c r="BO14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45279</v>
+        <v>45280</v>
       </c>
       <c r="BR14" s="159" t="s">
         <v>44</v>
@@ -5169,7 +5203,7 @@
       <c r="CF14" s="43"/>
       <c r="CG14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45279</v>
+        <v>45280</v>
       </c>
     </row>
     <row r="15" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6792,6 +6826,46 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
+      <c r="R26" s="173" t="s">
+        <v>145</v>
+      </c>
+      <c r="S26" s="174"/>
+      <c r="T26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="U26" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="V26" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="W26" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="X26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y26" s="125" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z26" s="125" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA26" s="153" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB26" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="AC26" s="157" t="s">
+        <v>83</v>
+      </c>
+      <c r="AD26" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE26" s="26" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="27" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="136"/>
@@ -6806,6 +6880,18 @@
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
       <c r="O27" s="101"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="2"/>
+      <c r="U27" s="25"/>
+      <c r="V27" s="117"/>
+      <c r="W27" s="2"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="152"/>
+      <c r="AB27" s="1"/>
+      <c r="AC27" s="1"/>
+      <c r="AD27" s="1"/>
+      <c r="AE27" s="25"/>
     </row>
     <row r="28" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="161">
@@ -6846,6 +6932,44 @@
       <c r="O28" s="101" t="s">
         <v>138</v>
       </c>
+      <c r="R28" s="161">
+        <v>10</v>
+      </c>
+      <c r="S28" s="37">
+        <v>10</v>
+      </c>
+      <c r="T28" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="U28" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="V28" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="W28" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="X28" s="143" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y28" s="145" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z28" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA28" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AB28" s="1"/>
+      <c r="AC28" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AD28" s="1"/>
+      <c r="AE28" s="25" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="29" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="133">
@@ -6886,6 +7010,44 @@
       <c r="O29" s="101" t="s">
         <v>138</v>
       </c>
+      <c r="R29" s="133">
+        <v>20</v>
+      </c>
+      <c r="S29" s="126">
+        <v>20</v>
+      </c>
+      <c r="T29" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="U29" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="V29" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="W29" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="X29" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y29" s="147" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z29" s="148" t="s">
+        <v>86</v>
+      </c>
+      <c r="AA29" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AD29" s="1"/>
+      <c r="AE29" s="25" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="30" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="133">
@@ -6925,6 +7087,44 @@
       <c r="N30" s="1"/>
       <c r="O30" s="101" t="s">
         <v>138</v>
+      </c>
+      <c r="R30" s="133">
+        <v>5</v>
+      </c>
+      <c r="S30" s="127">
+        <v>20</v>
+      </c>
+      <c r="T30" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="U30" s="120" t="s">
+        <v>17</v>
+      </c>
+      <c r="V30" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="W30" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="X30" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y30" s="145" t="s">
+        <v>96</v>
+      </c>
+      <c r="Z30" s="148" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA30" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AD30" s="1"/>
+      <c r="AE30" s="25" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6965,6 +7165,44 @@
       <c r="N31" s="1"/>
       <c r="O31" s="101" t="s">
         <v>138</v>
+      </c>
+      <c r="R31" s="140">
+        <v>5</v>
+      </c>
+      <c r="S31" s="127"/>
+      <c r="T31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="U31" s="124" t="s">
+        <v>17</v>
+      </c>
+      <c r="V31" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="W31" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="X31" s="143" t="s">
+        <v>91</v>
+      </c>
+      <c r="Y31" s="149" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z31" s="148" t="s">
+        <v>90</v>
+      </c>
+      <c r="AA31" s="154">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC31" s="154">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="AD31" s="1"/>
+      <c r="AE31" s="25" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7004,8 +7242,44 @@
       <c r="O32" s="101" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R32" s="33"/>
+      <c r="S32" s="37">
+        <v>10</v>
+      </c>
+      <c r="T32" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="U32" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="V32" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="W32" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="X32" s="143" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y32" s="149" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z32" s="148" t="s">
+        <v>69</v>
+      </c>
+      <c r="AA32" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AD32" s="1"/>
+      <c r="AE32" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="33"/>
       <c r="C33" s="126">
         <v>25</v>
@@ -7040,8 +7314,44 @@
       <c r="O33" s="101" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R33" s="33"/>
+      <c r="S33" s="126">
+        <v>10</v>
+      </c>
+      <c r="T33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="U33" s="156" t="s">
+        <v>17</v>
+      </c>
+      <c r="V33" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="W33" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="X33" s="143" t="s">
+        <v>129</v>
+      </c>
+      <c r="Y33" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z33" s="148" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA33" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AB33" s="1"/>
+      <c r="AC33" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AD33" s="1"/>
+      <c r="AE33" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="33"/>
       <c r="C34" s="37">
         <v>12</v>
@@ -7078,8 +7388,46 @@
       <c r="O34" s="101" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R34" s="33">
+        <v>70</v>
+      </c>
+      <c r="S34" s="37"/>
+      <c r="T34" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="U34" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="V34" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="W34" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="X34" s="144" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y34" s="149" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z34" s="148" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA34" s="154">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC34" s="154">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="AD34" s="1"/>
+      <c r="AE34" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="140">
         <v>100</v>
       </c>
@@ -7118,8 +7466,44 @@
       <c r="O35" s="101" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="R35" s="140"/>
+      <c r="S35" s="37">
+        <v>2</v>
+      </c>
+      <c r="T35" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="U35" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="V35" s="118" t="s">
+        <v>116</v>
+      </c>
+      <c r="W35" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="X35" s="143" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y35" s="150" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z35" s="151" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA35" s="154">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="AB35" s="1"/>
+      <c r="AC35" s="154">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="AD35" s="1"/>
+      <c r="AE35" s="25" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="36" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="171" t="s">
         <v>4</v>
       </c>
@@ -7141,14 +7525,33 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
+      <c r="R36" s="171" t="s">
+        <v>4</v>
+      </c>
+      <c r="S36" s="172"/>
+      <c r="T36" s="9">
+        <f>SUM(R28:S35)</f>
+        <v>182</v>
+      </c>
+      <c r="U36" s="25"/>
+      <c r="V36" s="117"/>
+      <c r="W36" s="2"/>
+      <c r="Y36" s="30"/>
+      <c r="AA36" s="155"/>
+      <c r="AB36" s="24"/>
+      <c r="AC36" s="1"/>
+      <c r="AD36" s="1"/>
+      <c r="AE36" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
     <mergeCell ref="BR24:BS24"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B36:C36"/>
+    <mergeCell ref="R26:S26"/>
+    <mergeCell ref="R36:S36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Update _22122023
Boat Enabled : 10:36 AM 22/12/2023
[3M] [28F Reserved] - [1F Mapped]

Boat Matrix - [-12]yd + [-1]td + (-3)ed
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6C9733-43D2-40DA-A050-ABAE00B89C27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E9B5B13-A161-4EC1-8D78-57F12614F606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1045" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="153">
   <si>
     <t>UnSettled</t>
   </si>
@@ -489,13 +489,19 @@
   </si>
   <si>
     <t>22/12/2023</t>
+  </si>
+  <si>
+    <t>23/12/2023</t>
+  </si>
+  <si>
+    <t>Bol News</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -624,6 +630,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="12">
     <fill>
@@ -1265,7 +1279,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1684,42 +1698,24 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1750,11 +1746,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2039,7 +2075,7 @@
   <dimension ref="A1:T19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="J13" sqref="J13:J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2060,7 +2096,7 @@
     <col min="15" max="15" width="4.85546875" style="1" customWidth="1"/>
     <col min="16" max="16" width="9" style="1" customWidth="1"/>
     <col min="17" max="17" width="2.85546875" style="1" customWidth="1"/>
-    <col min="18" max="18" width="11.140625" style="25" customWidth="1"/>
+    <col min="18" max="18" width="11.140625" style="24" customWidth="1"/>
     <col min="19" max="19" width="5.140625" customWidth="1"/>
     <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -2075,7 +2111,7 @@
       </c>
       <c r="C2" s="171">
         <f>B3+B4</f>
-        <v>271</v>
+        <v>91</v>
       </c>
       <c r="E2" s="175" t="s">
         <v>145</v>
@@ -2114,12 +2150,12 @@
       <c r="Q2" s="100" t="s">
         <v>36</v>
       </c>
-      <c r="R2" s="26" t="s">
+      <c r="R2" s="36" t="s">
         <v>108</v>
       </c>
       <c r="T2" s="98">
         <f ca="1">TODAY()</f>
-        <v>45281</v>
+        <v>45282</v>
       </c>
     </row>
     <row r="3" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2135,15 +2171,15 @@
     <row r="4" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="170"/>
       <c r="B4" s="34">
-        <v>271</v>
+        <v>91</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="161"/>
-      <c r="F4" s="165">
+      <c r="E4" s="140">
         <v>10</v>
       </c>
+      <c r="F4" s="165"/>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -2166,12 +2202,12 @@
         <v>30</v>
       </c>
       <c r="N4" s="154">
-        <v>0.79166666666666663</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="P4" s="154">
         <v>0.8208333333333333</v>
       </c>
-      <c r="R4" s="25" t="s">
+      <c r="R4" s="24" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2179,12 +2215,10 @@
       <c r="D5" s="157">
         <v>-2</v>
       </c>
-      <c r="E5" s="133">
-        <v>25</v>
-      </c>
-      <c r="F5" s="126">
-        <v>30</v>
-      </c>
+      <c r="E5" s="213">
+        <v>10</v>
+      </c>
+      <c r="F5" s="126"/>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2207,20 +2241,20 @@
         <v>86</v>
       </c>
       <c r="N5" s="154">
-        <v>0.79166666666666663</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="P5" s="154">
         <v>0.8208333333333333</v>
       </c>
-      <c r="R5" s="25" t="s">
+      <c r="R5" s="24" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="133"/>
-      <c r="F6" s="127">
-        <v>20</v>
-      </c>
+      <c r="E6" s="213">
+        <v>10</v>
+      </c>
+      <c r="F6" s="127"/>
       <c r="G6" s="28" t="s">
         <v>147</v>
       </c>
@@ -2243,12 +2277,12 @@
         <v>64</v>
       </c>
       <c r="N6" s="154">
-        <v>0.79166666666666663</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="P6" s="154">
         <v>0.8208333333333333</v>
       </c>
-      <c r="R6" s="25" t="s">
+      <c r="R6" s="24" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2259,10 +2293,10 @@
       <c r="B7" s="29">
         <v>0</v>
       </c>
-      <c r="E7" s="140"/>
-      <c r="F7" s="127">
+      <c r="E7" s="140">
         <v>10</v>
       </c>
+      <c r="F7" s="127"/>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2285,7 +2319,7 @@
         <v>90</v>
       </c>
       <c r="N7" s="154">
-        <v>0.79166666666666663</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="O7" s="1" t="s">
         <v>130</v>
@@ -2293,17 +2327,15 @@
       <c r="P7" s="154">
         <v>0.78472222222222221</v>
       </c>
-      <c r="R7" s="25" t="s">
+      <c r="R7" s="24" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="164">
-        <v>25</v>
-      </c>
-      <c r="F8" s="177">
-        <v>70</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="F8" s="177"/>
       <c r="G8" s="9" t="s">
         <v>72</v>
       </c>
@@ -2326,13 +2358,13 @@
         <v>69</v>
       </c>
       <c r="N8" s="154">
-        <v>0.4861111111111111</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="P8" s="154">
         <v>0.79166666666666663</v>
       </c>
-      <c r="R8" s="25" t="s">
-        <v>150</v>
+      <c r="R8" s="24" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2341,9 +2373,11 @@
       </c>
       <c r="B9" s="8">
         <f>7000-C2</f>
-        <v>6729</v>
-      </c>
-      <c r="E9" s="164"/>
+        <v>6909</v>
+      </c>
+      <c r="E9" s="140">
+        <v>10</v>
+      </c>
       <c r="F9" s="178"/>
       <c r="G9" s="9" t="s">
         <v>71</v>
@@ -2355,7 +2389,7 @@
         <v>115</v>
       </c>
       <c r="J9" s="33" t="s">
-        <v>140</v>
+        <v>21</v>
       </c>
       <c r="K9" s="143" t="s">
         <v>129</v>
@@ -2367,17 +2401,19 @@
         <v>64</v>
       </c>
       <c r="N9" s="154">
-        <v>0.79166666666666663</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="P9" s="154">
         <v>0.79166666666666663</v>
       </c>
-      <c r="R9" s="25" t="s">
-        <v>150</v>
+      <c r="R9" s="24" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="140"/>
+      <c r="E10" s="212">
+        <v>70</v>
+      </c>
       <c r="F10" s="179"/>
       <c r="G10" s="9" t="s">
         <v>81</v>
@@ -2401,16 +2437,16 @@
         <v>66</v>
       </c>
       <c r="N10" s="154">
-        <v>0.79166666666666663</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>126</v>
       </c>
       <c r="P10" s="154">
-        <v>0.4826388888888889</v>
-      </c>
-      <c r="R10" s="25" t="s">
-        <v>150</v>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="R10" s="24" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2421,10 +2457,10 @@
         <f>B9-B13</f>
         <v>0</v>
       </c>
-      <c r="E11" s="140"/>
-      <c r="F11" s="165">
+      <c r="E11" s="140">
         <v>10</v>
       </c>
+      <c r="F11" s="165"/>
       <c r="G11" s="9" t="s">
         <v>128</v>
       </c>
@@ -2435,7 +2471,7 @@
         <v>116</v>
       </c>
       <c r="J11" s="37" t="s">
-        <v>142</v>
+        <v>152</v>
       </c>
       <c r="K11" s="143" t="s">
         <v>110</v>
@@ -2447,12 +2483,12 @@
         <v>66</v>
       </c>
       <c r="N11" s="154">
-        <v>0.79166666666666663</v>
+        <v>0.43402777777777773</v>
       </c>
       <c r="P11" s="154">
         <v>0.80555555555555547</v>
       </c>
-      <c r="R11" s="25" t="s">
+      <c r="R11" s="24" t="s">
         <v>150</v>
       </c>
     </row>
@@ -2463,7 +2499,7 @@
       <c r="F12" s="174"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>200</v>
+        <v>180</v>
       </c>
       <c r="L12" s="30"/>
       <c r="M12"/>
@@ -2476,7 +2512,7 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>6729</v>
+        <v>6909</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="119"/>
@@ -2579,10 +2615,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N32" sqref="N32"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2606,18 +2642,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="180" t="s">
+      <c r="E1" s="196" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="181"/>
+      <c r="F1" s="197"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="180" t="s">
+      <c r="H1" s="196" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="182"/>
-      <c r="J1" s="181"/>
+      <c r="I1" s="198"/>
+      <c r="J1" s="197"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2662,26 +2698,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="186">
+      <c r="K2" s="199">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="188">
+      <c r="L2" s="201">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="192">
+      <c r="M2" s="186">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J34)</f>
-        <v>6689</v>
+        <f>SUM(E2:J35)</f>
+        <v>6869</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="184"/>
+      <c r="B3" s="185"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2696,13 +2732,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="187"/>
-      <c r="L3" s="189"/>
-      <c r="M3" s="193"/>
+      <c r="K3" s="200"/>
+      <c r="L3" s="202"/>
+      <c r="M3" s="187"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="185"/>
+      <c r="B4" s="184"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2717,9 +2753,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="187"/>
-      <c r="L4" s="189"/>
-      <c r="M4" s="193"/>
+      <c r="K4" s="200"/>
+      <c r="L4" s="202"/>
+      <c r="M4" s="187"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2801,7 +2837,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="194">
+      <c r="B7" s="188">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2818,22 +2854,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="196">
+      <c r="K7" s="190">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="198">
+      <c r="L7" s="192">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="200">
+      <c r="M7" s="194">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="195"/>
+      <c r="B8" s="189"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2854,9 +2890,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="197"/>
-      <c r="L8" s="199"/>
-      <c r="M8" s="201"/>
+      <c r="K8" s="191"/>
+      <c r="L8" s="193"/>
+      <c r="M8" s="195"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2936,7 +2972,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="194">
+      <c r="B11" s="188">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -2963,7 +2999,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="195"/>
+      <c r="B12" s="189"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -3020,7 +3056,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="194">
+      <c r="B14" s="188">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -3043,7 +3079,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="195"/>
+      <c r="B15" s="189"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3098,7 +3134,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="184"/>
+      <c r="B17" s="185"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3145,7 +3181,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="185"/>
+      <c r="B19" s="184"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3205,7 +3241,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="190">
+      <c r="B21" s="181">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3233,7 +3269,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="191"/>
+      <c r="B22" s="182"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -3373,7 +3409,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="203"/>
+      <c r="B27" s="180"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -3524,8 +3560,8 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="202"/>
-      <c r="C33" s="18"/>
+      <c r="B33" s="172"/>
+      <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
       <c r="F33" s="18">
@@ -3548,38 +3584,62 @@
       <c r="M33" s="18"/>
     </row>
     <row r="34" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="130">
+      <c r="B34" s="34">
         <v>21</v>
       </c>
-      <c r="C34" s="18"/>
-      <c r="D34" s="18"/>
-      <c r="E34" s="18"/>
-      <c r="F34" s="18">
+      <c r="C34" s="96"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82">
         <v>50</v>
       </c>
-      <c r="G34" s="18">
+      <c r="G34" s="82">
         <v>70</v>
       </c>
-      <c r="H34" s="18">
+      <c r="H34" s="82">
         <v>30</v>
       </c>
-      <c r="I34" s="18">
+      <c r="I34" s="82">
         <v>20</v>
       </c>
-      <c r="J34" s="18">
+      <c r="J34" s="82">
         <v>30</v>
       </c>
-      <c r="K34" s="18"/>
-      <c r="L34" s="18"/>
-      <c r="M34" s="18"/>
+      <c r="K34" s="82"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="82"/>
+    </row>
+    <row r="35" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="34">
+        <v>22</v>
+      </c>
+      <c r="C35" s="142"/>
+      <c r="D35" s="18"/>
+      <c r="E35" s="18"/>
+      <c r="F35" s="211">
+        <v>50</v>
+      </c>
+      <c r="G35" s="211">
+        <v>70</v>
+      </c>
+      <c r="H35" s="211">
+        <v>40</v>
+      </c>
+      <c r="I35" s="18"/>
+      <c r="J35" s="211">
+        <v>20</v>
+      </c>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="K2:K4"/>
+    <mergeCell ref="L2:L4"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B16:B17"/>
@@ -3590,11 +3650,11 @@
     <mergeCell ref="L7:L8"/>
     <mergeCell ref="M7:M8"/>
     <mergeCell ref="B7:B8"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="K2:K4"/>
-    <mergeCell ref="L2:L4"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3604,8 +3664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6EF39B9-450C-4C51-9807-7AFD5CC29C14}">
   <dimension ref="A1:CG36"/>
   <sheetViews>
-    <sheetView topLeftCell="AC19" workbookViewId="0">
-      <selection activeCell="AS37" sqref="AS37"/>
+    <sheetView topLeftCell="AS19" workbookViewId="0">
+      <selection activeCell="BH38" sqref="BH38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5155,7 +5215,7 @@
       </c>
       <c r="AC14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45281</v>
+        <v>45282</v>
       </c>
       <c r="AG14" s="99" t="s">
         <v>44</v>
@@ -5200,7 +5260,7 @@
       <c r="AU14" s="43"/>
       <c r="AV14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45281</v>
+        <v>45282</v>
       </c>
       <c r="AZ14" s="99" t="s">
         <v>44</v>
@@ -5245,7 +5305,7 @@
       <c r="BN14" s="43"/>
       <c r="BO14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45281</v>
+        <v>45282</v>
       </c>
       <c r="BR14" s="159" t="s">
         <v>44</v>
@@ -5290,7 +5350,7 @@
       <c r="CF14" s="43"/>
       <c r="CG14" s="98">
         <f ca="1">TODAY()</f>
-        <v>45281</v>
+        <v>45282</v>
       </c>
     </row>
     <row r="15" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6993,6 +7053,46 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
+      <c r="AW26" s="175" t="s">
+        <v>145</v>
+      </c>
+      <c r="AX26" s="176"/>
+      <c r="AY26" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="AZ26" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="BA26" s="83" t="s">
+        <v>41</v>
+      </c>
+      <c r="BB26" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="BC26" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="BD26" s="125" t="s">
+        <v>38</v>
+      </c>
+      <c r="BE26" s="125" t="s">
+        <v>92</v>
+      </c>
+      <c r="BF26" s="153" t="s">
+        <v>68</v>
+      </c>
+      <c r="BG26" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="BH26" s="157" t="s">
+        <v>83</v>
+      </c>
+      <c r="BI26" s="100" t="s">
+        <v>36</v>
+      </c>
+      <c r="BJ26" s="26" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="27" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="136"/>
@@ -7031,6 +7131,20 @@
       <c r="AR27" s="1"/>
       <c r="AS27" s="1"/>
       <c r="AT27" s="101"/>
+      <c r="AW27" s="136"/>
+      <c r="AX27" s="203"/>
+      <c r="AY27" s="204"/>
+      <c r="AZ27" s="205"/>
+      <c r="BA27" s="206"/>
+      <c r="BB27" s="203"/>
+      <c r="BC27" s="204"/>
+      <c r="BD27" s="207"/>
+      <c r="BE27" s="207"/>
+      <c r="BF27" s="208"/>
+      <c r="BG27" s="207"/>
+      <c r="BH27" s="207"/>
+      <c r="BI27" s="207"/>
+      <c r="BJ27" s="101"/>
     </row>
     <row r="28" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="161">
@@ -7147,6 +7261,42 @@
       <c r="AT28" s="101" t="s">
         <v>148</v>
       </c>
+      <c r="AW28" s="161"/>
+      <c r="AX28" s="165">
+        <v>10</v>
+      </c>
+      <c r="AY28" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AZ28" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA28" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB28" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="BC28" s="143" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD28" s="145" t="s">
+        <v>146</v>
+      </c>
+      <c r="BE28" s="146" t="s">
+        <v>30</v>
+      </c>
+      <c r="BF28" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BG28" s="207"/>
+      <c r="BH28" s="209">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="BI28" s="207"/>
+      <c r="BJ28" s="101" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="29" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="133">
@@ -7263,6 +7413,44 @@
       <c r="AT29" s="101" t="s">
         <v>148</v>
       </c>
+      <c r="AW29" s="133">
+        <v>25</v>
+      </c>
+      <c r="AX29" s="126">
+        <v>30</v>
+      </c>
+      <c r="AY29" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="AZ29" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA29" s="83" t="s">
+        <v>113</v>
+      </c>
+      <c r="BB29" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="BC29" s="143" t="s">
+        <v>119</v>
+      </c>
+      <c r="BD29" s="147" t="s">
+        <v>137</v>
+      </c>
+      <c r="BE29" s="148" t="s">
+        <v>86</v>
+      </c>
+      <c r="BF29" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BG29" s="207"/>
+      <c r="BH29" s="209">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="BI29" s="207"/>
+      <c r="BJ29" s="101" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="30" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="133">
@@ -7378,6 +7566,42 @@
       <c r="AS30" s="1"/>
       <c r="AT30" s="101" t="s">
         <v>148</v>
+      </c>
+      <c r="AW30" s="133"/>
+      <c r="AX30" s="127">
+        <v>20</v>
+      </c>
+      <c r="AY30" s="210" t="s">
+        <v>147</v>
+      </c>
+      <c r="AZ30" s="120" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA30" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="BB30" s="37" t="s">
+        <v>133</v>
+      </c>
+      <c r="BC30" s="143" t="s">
+        <v>120</v>
+      </c>
+      <c r="BD30" s="145" t="s">
+        <v>96</v>
+      </c>
+      <c r="BE30" s="148" t="s">
+        <v>64</v>
+      </c>
+      <c r="BF30" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BG30" s="207"/>
+      <c r="BH30" s="209">
+        <v>0.8208333333333333</v>
+      </c>
+      <c r="BI30" s="207"/>
+      <c r="BJ30" s="101" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7496,6 +7720,44 @@
       <c r="AS31" s="1"/>
       <c r="AT31" s="101" t="s">
         <v>148</v>
+      </c>
+      <c r="AW31" s="140"/>
+      <c r="AX31" s="127">
+        <v>10</v>
+      </c>
+      <c r="AY31" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="AZ31" s="124" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA31" s="83" t="s">
+        <v>105</v>
+      </c>
+      <c r="BB31" s="37" t="s">
+        <v>137</v>
+      </c>
+      <c r="BC31" s="143" t="s">
+        <v>149</v>
+      </c>
+      <c r="BD31" s="149" t="s">
+        <v>85</v>
+      </c>
+      <c r="BE31" s="148" t="s">
+        <v>90</v>
+      </c>
+      <c r="BF31" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BG31" s="207" t="s">
+        <v>130</v>
+      </c>
+      <c r="BH31" s="209">
+        <v>0.78472222222222221</v>
+      </c>
+      <c r="BI31" s="207"/>
+      <c r="BJ31" s="101" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7607,8 +7869,46 @@
       <c r="AT32" s="101" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="33" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AW32" s="164">
+        <v>25</v>
+      </c>
+      <c r="AX32" s="177">
+        <v>70</v>
+      </c>
+      <c r="AY32" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="AZ32" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA32" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="BB32" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="BC32" s="143" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD32" s="149" t="s">
+        <v>123</v>
+      </c>
+      <c r="BE32" s="148" t="s">
+        <v>69</v>
+      </c>
+      <c r="BF32" s="209">
+        <v>0.4861111111111111</v>
+      </c>
+      <c r="BG32" s="207"/>
+      <c r="BH32" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BI32" s="207"/>
+      <c r="BJ32" s="101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="33"/>
       <c r="C33" s="126">
         <v>25</v>
@@ -7717,8 +8017,42 @@
       <c r="AT33" s="101" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="34" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AW33" s="164"/>
+      <c r="AX33" s="178"/>
+      <c r="AY33" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="AZ33" s="156" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA33" s="83" t="s">
+        <v>115</v>
+      </c>
+      <c r="BB33" s="33" t="s">
+        <v>140</v>
+      </c>
+      <c r="BC33" s="143" t="s">
+        <v>129</v>
+      </c>
+      <c r="BD33" s="149" t="s">
+        <v>78</v>
+      </c>
+      <c r="BE33" s="148" t="s">
+        <v>64</v>
+      </c>
+      <c r="BF33" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BG33" s="207"/>
+      <c r="BH33" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BI33" s="207"/>
+      <c r="BJ33" s="101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="34" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="33"/>
       <c r="C34" s="37">
         <v>12</v>
@@ -7833,8 +8167,44 @@
       <c r="AT34" s="101" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="35" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AW34" s="140"/>
+      <c r="AX34" s="179"/>
+      <c r="AY34" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AZ34" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA34" s="83" t="s">
+        <v>32</v>
+      </c>
+      <c r="BB34" s="37" t="s">
+        <v>94</v>
+      </c>
+      <c r="BC34" s="144" t="s">
+        <v>122</v>
+      </c>
+      <c r="BD34" s="149" t="s">
+        <v>124</v>
+      </c>
+      <c r="BE34" s="148" t="s">
+        <v>66</v>
+      </c>
+      <c r="BF34" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BG34" s="207" t="s">
+        <v>126</v>
+      </c>
+      <c r="BH34" s="209">
+        <v>0.4826388888888889</v>
+      </c>
+      <c r="BI34" s="207"/>
+      <c r="BJ34" s="101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="35" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="140">
         <v>100</v>
       </c>
@@ -7947,8 +8317,44 @@
       <c r="AT35" s="101" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="36" spans="2:46" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AW35" s="140"/>
+      <c r="AX35" s="165">
+        <v>10</v>
+      </c>
+      <c r="AY35" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="AZ35" s="107" t="s">
+        <v>17</v>
+      </c>
+      <c r="BA35" s="118" t="s">
+        <v>116</v>
+      </c>
+      <c r="BB35" s="37" t="s">
+        <v>142</v>
+      </c>
+      <c r="BC35" s="143" t="s">
+        <v>110</v>
+      </c>
+      <c r="BD35" s="150" t="s">
+        <v>143</v>
+      </c>
+      <c r="BE35" s="151" t="s">
+        <v>66</v>
+      </c>
+      <c r="BF35" s="209">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="BG35" s="207"/>
+      <c r="BH35" s="209">
+        <v>0.80555555555555547</v>
+      </c>
+      <c r="BI35" s="207"/>
+      <c r="BJ35" s="101" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="36" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B36" s="173" t="s">
         <v>4</v>
       </c>
@@ -8012,9 +8418,30 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
+      <c r="AW36" s="173" t="s">
+        <v>4</v>
+      </c>
+      <c r="AX36" s="174"/>
+      <c r="AY36" s="9">
+        <f>SUM(AW28:AX35)</f>
+        <v>200</v>
+      </c>
+      <c r="AZ36" s="114"/>
+      <c r="BA36" s="137"/>
+      <c r="BB36" s="79"/>
+      <c r="BC36" s="50"/>
+      <c r="BD36" s="138"/>
+      <c r="BE36" s="50"/>
+      <c r="BF36" s="158"/>
+      <c r="BG36" s="115" t="s">
+        <v>148</v>
+      </c>
+      <c r="BH36" s="65"/>
+      <c r="BI36" s="65"/>
+      <c r="BJ36" s="102"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
     <mergeCell ref="AG24:AH24"/>
     <mergeCell ref="AZ24:BA24"/>
     <mergeCell ref="BR24:BS24"/>
@@ -8024,6 +8451,9 @@
     <mergeCell ref="R36:S36"/>
     <mergeCell ref="AG26:AH26"/>
     <mergeCell ref="AG36:AH36"/>
+    <mergeCell ref="AW26:AX26"/>
+    <mergeCell ref="AX32:AX34"/>
+    <mergeCell ref="AW36:AX36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Rw Usage Updates _18:48
Rw Usage Updates _18:48
Reserved Wbt For Tomorrow :- 12
Reserved for Host :- 8
Node :- ED(-3)
Deployed(27 F) :- BirdW(12) + FuelW(15)
</commit_message>
<xml_diff>
--- a/Usage_S_1.0.4.xlsx
+++ b/Usage_S_1.0.4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Work_For_\Work\Running AppS\System_Work_RW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73AD953E-6463-4B5D-B485-31A4AE7F0EC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5BF1C16-5669-48BB-9C3C-CD867001DE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1130" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1133" uniqueCount="159">
   <si>
     <t>UnSettled</t>
   </si>
@@ -498,6 +498,21 @@
   </si>
   <si>
     <t xml:space="preserve">World Desk </t>
+  </si>
+  <si>
+    <t>ND TV 24*7</t>
+  </si>
+  <si>
+    <t>Sky News A</t>
+  </si>
+  <si>
+    <t>India TV</t>
+  </si>
+  <si>
+    <t>PTM News</t>
+  </si>
+  <si>
+    <t>France 24 ES</t>
   </si>
 </sst>
 </file>
@@ -710,7 +725,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="45">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -1278,11 +1293,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="205">
+  <cellXfs count="207">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1665,6 +1695,9 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1775,6 +1808,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2059,7 +2095,7 @@
   <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2072,7 +2108,7 @@
     <col min="7" max="7" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="3.5703125" style="25" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" style="117" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.85546875" style="117" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.140625" style="117" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.42578125" style="1" customWidth="1"/>
@@ -2094,14 +2130,14 @@
       <c r="B2" s="34">
         <v>40.380000000000003</v>
       </c>
-      <c r="C2" s="173">
+      <c r="C2" s="174">
         <f>B3+B4</f>
-        <v>91</v>
-      </c>
-      <c r="E2" s="177" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="F2" s="178"/>
+      <c r="F2" s="179"/>
       <c r="G2" s="26" t="s">
         <v>43</v>
       </c>
@@ -2147,19 +2183,19 @@
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="171" t="s">
+      <c r="A3" s="172" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="34"/>
-      <c r="C3" s="174"/>
+      <c r="C3" s="175"/>
       <c r="D3" s="163" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="172"/>
+      <c r="A4" s="173"/>
       <c r="B4" s="34">
-        <v>91</v>
+        <v>11</v>
       </c>
       <c r="C4" s="33" t="s">
         <v>35</v>
@@ -2167,7 +2203,9 @@
       <c r="E4" s="140">
         <v>10</v>
       </c>
-      <c r="F4" s="165"/>
+      <c r="F4" s="165">
+        <v>10</v>
+      </c>
       <c r="G4" s="9" t="s">
         <v>1</v>
       </c>
@@ -2187,19 +2225,19 @@
         <v>118</v>
       </c>
       <c r="M4" s="145" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="N4" s="146" t="s">
         <v>30</v>
       </c>
       <c r="O4" s="154">
-        <v>0.43402777777777773</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="Q4" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="S4" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2209,7 +2247,9 @@
       <c r="E5" s="167">
         <v>10</v>
       </c>
-      <c r="F5" s="126"/>
+      <c r="F5" s="126">
+        <v>10</v>
+      </c>
       <c r="G5" s="9" t="s">
         <v>136</v>
       </c>
@@ -2219,7 +2259,9 @@
       <c r="I5" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="J5" s="83"/>
+      <c r="J5" s="206" t="s">
+        <v>157</v>
+      </c>
       <c r="K5" s="37" t="s">
         <v>85</v>
       </c>
@@ -2233,33 +2275,35 @@
         <v>86</v>
       </c>
       <c r="O5" s="154">
-        <v>0.43402777777777773</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="Q5" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="S5" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E6" s="167">
         <v>10</v>
       </c>
-      <c r="F6" s="127"/>
+      <c r="F6" s="127">
+        <v>20</v>
+      </c>
       <c r="G6" s="28" t="s">
         <v>147</v>
       </c>
       <c r="H6" s="120" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="83" t="s">
-        <v>115</v>
-      </c>
+      <c r="I6" s="83"/>
       <c r="J6" s="83" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="83" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="37"/>
       <c r="L6" s="143" t="s">
         <v>120</v>
       </c>
@@ -2270,13 +2314,13 @@
         <v>64</v>
       </c>
       <c r="O6" s="154">
-        <v>0.43402777777777773</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="Q6" s="154">
-        <v>0.8208333333333333</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="S6" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2289,7 +2333,9 @@
       <c r="E7" s="140">
         <v>10</v>
       </c>
-      <c r="F7" s="127"/>
+      <c r="F7" s="127">
+        <v>10</v>
+      </c>
       <c r="G7" s="9" t="s">
         <v>9</v>
       </c>
@@ -2299,9 +2345,11 @@
       <c r="I7" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="J7" s="83"/>
+      <c r="J7" s="83" t="s">
+        <v>137</v>
+      </c>
       <c r="K7" s="37" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="L7" s="143" t="s">
         <v>149</v>
@@ -2313,23 +2361,25 @@
         <v>90</v>
       </c>
       <c r="O7" s="154">
-        <v>0.43402777777777773</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="P7" s="1" t="s">
         <v>130</v>
       </c>
       <c r="Q7" s="154">
-        <v>0.78472222222222221</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="S7" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E8" s="164">
         <v>50</v>
       </c>
-      <c r="F8" s="179"/>
+      <c r="F8" s="180">
+        <v>20</v>
+      </c>
       <c r="G8" s="9" t="s">
         <v>72</v>
       </c>
@@ -2339,7 +2389,9 @@
       <c r="I8" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="J8" s="83"/>
+      <c r="J8" s="83" t="s">
+        <v>143</v>
+      </c>
       <c r="K8" s="33" t="s">
         <v>62</v>
       </c>
@@ -2368,22 +2420,22 @@
       </c>
       <c r="B9" s="8">
         <f>7000-C2</f>
-        <v>6909</v>
+        <v>6989</v>
       </c>
       <c r="E9" s="140">
         <v>10</v>
       </c>
-      <c r="F9" s="180"/>
+      <c r="F9" s="181"/>
       <c r="G9" s="9" t="s">
         <v>71</v>
       </c>
       <c r="H9" s="156" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="83" t="s">
-        <v>115</v>
-      </c>
-      <c r="J9" s="83"/>
+      <c r="I9" s="83"/>
+      <c r="J9" s="83" t="s">
+        <v>158</v>
+      </c>
       <c r="K9" s="33" t="s">
         <v>21</v>
       </c>
@@ -2410,7 +2462,7 @@
       <c r="E10" s="166">
         <v>70</v>
       </c>
-      <c r="F10" s="181"/>
+      <c r="F10" s="182"/>
       <c r="G10" s="9" t="s">
         <v>81</v>
       </c>
@@ -2459,7 +2511,9 @@
       <c r="E11" s="140">
         <v>10</v>
       </c>
-      <c r="F11" s="165"/>
+      <c r="F11" s="165">
+        <v>10</v>
+      </c>
       <c r="G11" s="9" t="s">
         <v>128</v>
       </c>
@@ -2485,23 +2539,23 @@
         <v>66</v>
       </c>
       <c r="O11" s="154">
-        <v>0.43402777777777773</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="Q11" s="154">
-        <v>0.80555555555555547</v>
+        <v>0.76388888888888884</v>
       </c>
       <c r="S11" s="24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E12" s="175" t="s">
+      <c r="E12" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="176"/>
+      <c r="F12" s="177"/>
       <c r="G12" s="9">
         <f>SUM(E4:F11)</f>
-        <v>180</v>
+        <v>260</v>
       </c>
       <c r="M12" s="30"/>
       <c r="N12"/>
@@ -2514,16 +2568,16 @@
       </c>
       <c r="B13" s="8">
         <f>B18+Purchase!O2</f>
-        <v>6909</v>
+        <v>6989</v>
       </c>
       <c r="G13" s="28"/>
       <c r="I13" s="119"/>
       <c r="J13" s="119"/>
-      <c r="K13" s="168"/>
+      <c r="K13" s="169"/>
       <c r="M13"/>
       <c r="N13"/>
-      <c r="O13" s="169"/>
-      <c r="P13" s="170"/>
+      <c r="O13" s="170"/>
+      <c r="P13" s="171"/>
     </row>
     <row r="14" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C14" s="25"/>
@@ -2532,11 +2586,11 @@
       <c r="F14" s="20"/>
       <c r="I14" s="119"/>
       <c r="J14" s="119"/>
-      <c r="K14" s="168"/>
+      <c r="K14" s="169"/>
       <c r="M14"/>
       <c r="N14"/>
-      <c r="O14" s="169"/>
-      <c r="P14" s="170"/>
+      <c r="O14" s="170"/>
+      <c r="P14" s="171"/>
     </row>
     <row r="15" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
@@ -2551,12 +2605,12 @@
       <c r="F15" s="20"/>
       <c r="I15" s="119"/>
       <c r="J15" s="119"/>
-      <c r="K15" s="168"/>
+      <c r="K15" s="169"/>
       <c r="L15" s="119"/>
       <c r="M15"/>
       <c r="N15"/>
-      <c r="O15" s="169"/>
-      <c r="P15" s="170"/>
+      <c r="O15" s="170"/>
+      <c r="P15" s="171"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C16" s="25"/>
@@ -2577,8 +2631,8 @@
       <c r="J17" s="119"/>
       <c r="M17"/>
       <c r="N17"/>
-      <c r="O17" s="169"/>
-      <c r="P17" s="170"/>
+      <c r="O17" s="170"/>
+      <c r="P17" s="171"/>
     </row>
     <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
@@ -2591,14 +2645,14 @@
       <c r="D18" s="25"/>
       <c r="E18" s="24"/>
       <c r="F18" s="20"/>
-      <c r="K18" s="168"/>
+      <c r="K18" s="169"/>
       <c r="M18"/>
       <c r="N18"/>
-      <c r="O18" s="169"/>
-      <c r="P18" s="170"/>
+      <c r="O18" s="170"/>
+      <c r="P18" s="171"/>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="K19" s="168"/>
+      <c r="K19" s="169"/>
       <c r="M19"/>
       <c r="N19"/>
     </row>
@@ -2622,7 +2676,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0951DD9-29CF-40D7-AA95-AE74BC805B9C}">
-  <dimension ref="A1:O35"/>
+  <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="O3" sqref="O3"/>
@@ -2649,18 +2703,18 @@
       <c r="D1" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="182" t="s">
+      <c r="E1" s="183" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="183"/>
+      <c r="F1" s="184"/>
       <c r="G1" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="182" t="s">
+      <c r="H1" s="183" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="184"/>
-      <c r="J1" s="183"/>
+      <c r="I1" s="185"/>
+      <c r="J1" s="184"/>
       <c r="K1" s="23" t="s">
         <v>8</v>
       </c>
@@ -2678,7 +2732,7 @@
       <c r="A2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="185">
+      <c r="B2" s="186">
         <v>2</v>
       </c>
       <c r="C2" s="12">
@@ -2705,26 +2759,26 @@
       <c r="J2" s="10">
         <v>20</v>
       </c>
-      <c r="K2" s="188">
+      <c r="K2" s="189">
         <f>SUM(F2:J4)</f>
         <v>312</v>
       </c>
-      <c r="L2" s="190">
+      <c r="L2" s="191">
         <f>SUM(E2:J4)</f>
         <v>1152</v>
       </c>
-      <c r="M2" s="194">
+      <c r="M2" s="195">
         <f>SUM(D2:D4)-L2</f>
         <v>348</v>
       </c>
       <c r="O2">
-        <f>SUM(E2:J35)</f>
-        <v>6869</v>
+        <f>SUM(E2:J36)</f>
+        <v>6949</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="186"/>
+      <c r="B3" s="187"/>
       <c r="C3" s="13">
         <v>350</v>
       </c>
@@ -2739,13 +2793,13 @@
       <c r="H3" s="18"/>
       <c r="I3" s="18"/>
       <c r="J3" s="55"/>
-      <c r="K3" s="189"/>
-      <c r="L3" s="191"/>
-      <c r="M3" s="195"/>
+      <c r="K3" s="190"/>
+      <c r="L3" s="192"/>
+      <c r="M3" s="196"/>
     </row>
     <row r="4" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
-      <c r="B4" s="187"/>
+      <c r="B4" s="188"/>
       <c r="C4" s="6"/>
       <c r="D4" s="5">
         <v>500</v>
@@ -2760,9 +2814,9 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="189"/>
-      <c r="L4" s="191"/>
-      <c r="M4" s="195"/>
+      <c r="K4" s="190"/>
+      <c r="L4" s="192"/>
+      <c r="M4" s="196"/>
     </row>
     <row r="5" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="20"/>
@@ -2844,7 +2898,7 @@
       <c r="A7" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="196">
+      <c r="B7" s="197">
         <v>5</v>
       </c>
       <c r="C7" s="12"/>
@@ -2861,22 +2915,22 @@
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="10"/>
-      <c r="K7" s="198">
+      <c r="K7" s="199">
         <f>SUM(F7:J8)</f>
         <v>270</v>
       </c>
-      <c r="L7" s="200">
+      <c r="L7" s="201">
         <f>SUM(E7:J8)</f>
         <v>340</v>
       </c>
-      <c r="M7" s="202">
+      <c r="M7" s="203">
         <f>D8-L7</f>
         <v>160</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="197"/>
+      <c r="B8" s="198"/>
       <c r="C8" s="6"/>
       <c r="D8" s="7">
         <v>500</v>
@@ -2897,9 +2951,9 @@
       <c r="J8" s="4">
         <v>10</v>
       </c>
-      <c r="K8" s="199"/>
-      <c r="L8" s="201"/>
-      <c r="M8" s="203"/>
+      <c r="K8" s="200"/>
+      <c r="L8" s="202"/>
+      <c r="M8" s="204"/>
     </row>
     <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
@@ -2979,7 +3033,7 @@
       <c r="A11" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B11" s="196">
+      <c r="B11" s="197">
         <v>8</v>
       </c>
       <c r="C11" s="68"/>
@@ -3006,7 +3060,7 @@
       <c r="M11" s="70"/>
     </row>
     <row r="12" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="197"/>
+      <c r="B12" s="198"/>
       <c r="C12" s="90">
         <v>483</v>
       </c>
@@ -3063,7 +3117,7 @@
       <c r="M13" s="82"/>
     </row>
     <row r="14" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="196">
+      <c r="B14" s="197">
         <v>10</v>
       </c>
       <c r="C14" s="95"/>
@@ -3086,7 +3140,7 @@
       <c r="A15" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B15" s="197"/>
+      <c r="B15" s="198"/>
       <c r="C15" s="96"/>
       <c r="D15" s="82">
         <v>175</v>
@@ -3110,7 +3164,7 @@
       <c r="M15" s="91"/>
     </row>
     <row r="16" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="185">
+      <c r="B16" s="186">
         <v>11</v>
       </c>
       <c r="C16" s="18"/>
@@ -3141,7 +3195,7 @@
       <c r="A17" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="186"/>
+      <c r="B17" s="187"/>
       <c r="C17" s="82"/>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -3159,7 +3213,7 @@
       <c r="M17" s="82"/>
     </row>
     <row r="18" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="185">
+      <c r="B18" s="186">
         <v>12</v>
       </c>
       <c r="C18" s="12"/>
@@ -3188,7 +3242,7 @@
       <c r="A19" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B19" s="187"/>
+      <c r="B19" s="188"/>
       <c r="C19" s="13"/>
       <c r="D19" s="18">
         <v>100</v>
@@ -3248,7 +3302,7 @@
       <c r="A21" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="192">
+      <c r="B21" s="193">
         <v>14</v>
       </c>
       <c r="C21" s="13"/>
@@ -3276,7 +3330,7 @@
       <c r="M21" s="55"/>
     </row>
     <row r="22" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="193"/>
+      <c r="B22" s="194"/>
       <c r="C22" s="131"/>
       <c r="D22" s="132">
         <v>235</v>
@@ -3328,7 +3382,7 @@
       <c r="M23" s="70"/>
     </row>
     <row r="24" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="173">
+      <c r="B24" s="174">
         <v>16</v>
       </c>
       <c r="C24" s="141"/>
@@ -3357,7 +3411,7 @@
       <c r="A25" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B25" s="174"/>
+      <c r="B25" s="175"/>
       <c r="C25" s="142"/>
       <c r="D25" s="18">
         <v>130</v>
@@ -3385,7 +3439,7 @@
       <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="173">
+      <c r="B26" s="174">
         <v>17</v>
       </c>
       <c r="C26" s="162"/>
@@ -3416,7 +3470,7 @@
       <c r="A27" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B27" s="204"/>
+      <c r="B27" s="205"/>
       <c r="C27" s="96"/>
       <c r="D27" s="132">
         <v>100</v>
@@ -3447,7 +3501,7 @@
       <c r="A28" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="173">
+      <c r="B28" s="174">
         <v>18</v>
       </c>
       <c r="C28" s="141"/>
@@ -3469,7 +3523,7 @@
       <c r="M28" s="70"/>
     </row>
     <row r="29" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="174"/>
+      <c r="B29" s="175"/>
       <c r="C29" s="142"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18">
@@ -3495,7 +3549,7 @@
       <c r="M29" s="18"/>
     </row>
     <row r="30" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="173">
+      <c r="B30" s="174">
         <v>19</v>
       </c>
       <c r="C30" s="142"/>
@@ -3518,7 +3572,7 @@
       <c r="A31" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B31" s="174"/>
+      <c r="B31" s="175"/>
       <c r="C31" s="142"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -3545,7 +3599,7 @@
       <c r="A32" s="84" t="s">
         <v>1</v>
       </c>
-      <c r="B32" s="173">
+      <c r="B32" s="174">
         <v>20</v>
       </c>
       <c r="C32" s="142"/>
@@ -3567,7 +3621,7 @@
       <c r="M32" s="18"/>
     </row>
     <row r="33" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="174"/>
+      <c r="B33" s="175"/>
       <c r="C33" s="142"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -3616,29 +3670,53 @@
       <c r="L34" s="82"/>
       <c r="M34" s="82"/>
     </row>
-    <row r="35" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="34">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B35" s="168">
         <v>22</v>
       </c>
-      <c r="C35" s="142"/>
-      <c r="D35" s="18"/>
-      <c r="E35" s="18"/>
-      <c r="F35" s="18">
+      <c r="C35" s="96"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82">
         <v>50</v>
       </c>
-      <c r="G35" s="18">
+      <c r="G35" s="82">
         <v>70</v>
       </c>
-      <c r="H35" s="18">
+      <c r="H35" s="82">
         <v>40</v>
       </c>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18">
+      <c r="I35" s="82"/>
+      <c r="J35" s="82">
         <v>20</v>
       </c>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="82"/>
+    </row>
+    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B36" s="17">
+        <v>23</v>
+      </c>
+      <c r="C36" s="18"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="18"/>
+      <c r="F36" s="18">
+        <v>20</v>
+      </c>
+      <c r="G36" s="18">
+        <v>20</v>
+      </c>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18">
+        <v>20</v>
+      </c>
+      <c r="J36" s="18">
+        <v>20</v>
+      </c>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="20">
@@ -6868,10 +6946,10 @@
       <c r="CG23" s="49"/>
     </row>
     <row r="24" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AG24" s="175" t="s">
+      <c r="AG24" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="AH24" s="176"/>
+      <c r="AH24" s="177"/>
       <c r="AI24" s="9">
         <f>SUM(AG16:AH23)</f>
         <v>40</v>
@@ -6891,10 +6969,10 @@
       <c r="AV24" s="51" t="s">
         <v>112</v>
       </c>
-      <c r="AZ24" s="175" t="s">
+      <c r="AZ24" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="BA24" s="176"/>
+      <c r="BA24" s="177"/>
       <c r="BB24" s="9">
         <f>SUM(AZ16:BA23)</f>
         <v>335</v>
@@ -6914,10 +6992,10 @@
       <c r="BO24" s="51" t="s">
         <v>127</v>
       </c>
-      <c r="BR24" s="175" t="s">
+      <c r="BR24" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="BS24" s="176"/>
+      <c r="BS24" s="177"/>
       <c r="BT24" s="9">
         <f>SUM(BR16:BS23)</f>
         <v>275</v>
@@ -6940,10 +7018,10 @@
     </row>
     <row r="25" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:85" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="177" t="s">
+      <c r="B26" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="C26" s="178"/>
+      <c r="C26" s="179"/>
       <c r="D26" s="26" t="s">
         <v>43</v>
       </c>
@@ -6980,10 +7058,10 @@
       <c r="O26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="R26" s="177" t="s">
+      <c r="R26" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="S26" s="178"/>
+      <c r="S26" s="179"/>
       <c r="T26" s="26" t="s">
         <v>43</v>
       </c>
@@ -7020,10 +7098,10 @@
       <c r="AE26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AG26" s="177" t="s">
+      <c r="AG26" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="AH26" s="178"/>
+      <c r="AH26" s="179"/>
       <c r="AI26" s="26" t="s">
         <v>43</v>
       </c>
@@ -7060,10 +7138,10 @@
       <c r="AT26" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="AW26" s="177" t="s">
+      <c r="AW26" s="178" t="s">
         <v>145</v>
       </c>
-      <c r="AX26" s="178"/>
+      <c r="AX26" s="179"/>
       <c r="AY26" s="26" t="s">
         <v>43</v>
       </c>
@@ -7877,7 +7955,7 @@
       <c r="AW32" s="164">
         <v>25</v>
       </c>
-      <c r="AX32" s="179">
+      <c r="AX32" s="180">
         <v>70</v>
       </c>
       <c r="AY32" s="9" t="s">
@@ -8023,7 +8101,7 @@
         <v>148</v>
       </c>
       <c r="AW33" s="164"/>
-      <c r="AX33" s="180"/>
+      <c r="AX33" s="181"/>
       <c r="AY33" s="9" t="s">
         <v>71</v>
       </c>
@@ -8173,7 +8251,7 @@
         <v>148</v>
       </c>
       <c r="AW34" s="140"/>
-      <c r="AX34" s="181"/>
+      <c r="AX34" s="182"/>
       <c r="AY34" s="9" t="s">
         <v>81</v>
       </c>
@@ -8360,10 +8438,10 @@
       </c>
     </row>
     <row r="36" spans="2:62" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="175" t="s">
+      <c r="B36" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="176"/>
+      <c r="C36" s="177"/>
       <c r="D36" s="9">
         <f>SUM(B28:C35)</f>
         <v>512</v>
@@ -8381,10 +8459,10 @@
       <c r="M36" s="65"/>
       <c r="N36" s="65"/>
       <c r="O36" s="102"/>
-      <c r="R36" s="175" t="s">
+      <c r="R36" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="S36" s="176"/>
+      <c r="S36" s="177"/>
       <c r="T36" s="9">
         <f>SUM(R28:S35)</f>
         <v>182</v>
@@ -8402,10 +8480,10 @@
       <c r="AC36" s="65"/>
       <c r="AD36" s="65"/>
       <c r="AE36" s="102"/>
-      <c r="AG36" s="175" t="s">
+      <c r="AG36" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="AH36" s="176"/>
+      <c r="AH36" s="177"/>
       <c r="AI36" s="9">
         <f>SUM(AG28:AH35)</f>
         <v>360</v>
@@ -8423,10 +8501,10 @@
       <c r="AR36" s="65"/>
       <c r="AS36" s="65"/>
       <c r="AT36" s="102"/>
-      <c r="AW36" s="175" t="s">
+      <c r="AW36" s="176" t="s">
         <v>4</v>
       </c>
-      <c r="AX36" s="176"/>
+      <c r="AX36" s="177"/>
       <c r="AY36" s="9">
         <f>SUM(AW28:AX35)</f>
         <v>200</v>

</xml_diff>